<commit_message>
remove e0 from INI and spreadsheet
make spreadsheet interpretation a bit more robust
</commit_message>
<xml_diff>
--- a/startup/wheel_template.xlsx
+++ b/startup/wheel_template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="46">
   <si>
     <t xml:space="preserve">Experimenters:</t>
   </si>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Scan numbers and plotting</t>
   </si>
   <si>
-    <t xml:space="preserve">Energy range</t>
+    <t xml:space="preserve">Photon delivery</t>
   </si>
   <si>
     <t xml:space="preserve">Sample metadata</t>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t xml:space="preserve">Plotting mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e0</t>
   </si>
   <si>
     <t xml:space="preserve">Element symbol</t>
@@ -242,7 +239,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -258,8 +255,22 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -311,18 +322,7 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right/>
-      <top style="thin">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FFCCCCCC"/>
-      </left>
+      <left style="hair"/>
       <right style="thin">
         <color rgb="FFCCCCCC"/>
       </right>
@@ -346,6 +346,28 @@
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="thin"/>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCCC"/>
+      </right>
       <top style="thin">
         <color rgb="FFCCCCCC"/>
       </top>
@@ -402,7 +424,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -443,6 +465,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -455,11 +481,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -467,7 +497,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -483,24 +513,16 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -515,23 +537,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -539,7 +561,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -551,7 +577,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -559,7 +585,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -567,7 +593,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -579,11 +605,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -595,7 +621,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -682,9 +708,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1228320</xdr:colOff>
+      <xdr:colOff>1227600</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>61920</xdr:rowOff>
+      <xdr:rowOff>61200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -698,7 +724,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="6933960"/>
-          <a:ext cx="2721240" cy="2745000"/>
+          <a:ext cx="2518560" cy="2744280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -718,10 +744,10 @@
       <xdr:rowOff>106560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>778320</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>919080</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>127080</xdr:rowOff>
+      <xdr:rowOff>126360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -730,8 +756,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3392280" y="6959880"/>
-          <a:ext cx="5859360" cy="1646280"/>
+          <a:off x="3190320" y="6959880"/>
+          <a:ext cx="4648320" cy="1645560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -921,25 +947,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:AA30"/>
+  <dimension ref="B1:AMJ30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="6" topLeftCell="O7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="6" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="O1" activeCellId="0" sqref="O1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="S7" activeCellId="0" sqref="S7"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="12" style="0" width="29.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="0" width="22.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="18" style="0" width="14.44"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="26" min="21" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="0" width="29.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="14" style="0" width="22.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="17" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="25" min="20" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="26" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -968,49 +1002,46 @@
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
       <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="5"/>
       <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="M2" s="6"/>
       <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="0"/>
       <c r="V2" s="0"/>
       <c r="W2" s="0"/>
       <c r="X2" s="0"/>
-      <c r="Y2" s="0"/>
-      <c r="Z2" s="5"/>
+      <c r="Y2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="5"/>
       <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="M3" s="6"/>
       <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="0"/>
       <c r="V3" s="0"/>
       <c r="W3" s="0"/>
       <c r="X3" s="0"/>
-      <c r="Y3" s="0"/>
-      <c r="Z3" s="5"/>
+      <c r="Y3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
@@ -1028,929 +1059,899 @@
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9" t="s">
+      <c r="K4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9" t="s">
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9" t="s">
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9" t="s">
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="V4" s="9"/>
-      <c r="W4" s="9"/>
-      <c r="X4" s="9"/>
-      <c r="Y4" s="9"/>
-      <c r="Z4" s="9"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="K5" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="M5" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="16" t="s">
+      <c r="N5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="O5" s="15" t="s">
+      <c r="O5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="P5" s="12" t="s">
+      <c r="P5" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="Q5" s="16" t="s">
+      <c r="Q5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="R5" s="17" t="s">
+      <c r="R5" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="S5" s="12" t="s">
+      <c r="S5" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="T5" s="16" t="s">
+      <c r="T5" s="12" t="s">
         <v>26</v>
       </c>
       <c r="U5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="V5" s="10" t="s">
+      <c r="V5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="W5" s="10" t="s">
+      <c r="W5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="X5" s="10" t="s">
+      <c r="X5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="Y5" s="10" t="s">
+      <c r="Y5" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="Z5" s="14" t="s">
+      <c r="Z5" s="20"/>
+    </row>
+    <row r="6" s="21" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B6" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="AA5" s="18"/>
-    </row>
-    <row r="6" s="19" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="E6" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="20" t="s">
+      <c r="G6" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="H6" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="24" t="n">
-        <v>8979</v>
-      </c>
-      <c r="I6" s="25" t="s">
+      <c r="I6" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="26" t="s">
+      <c r="J6" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="K6" s="27" t="s">
+      <c r="K6" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="28" t="s">
+      <c r="L6" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="M6" s="29" t="s">
+      <c r="M6" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="N6" s="30" t="s">
+      <c r="N6" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="O6" s="31" t="s">
+      <c r="O6" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="P6" s="32" t="s">
+      <c r="P6" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="Q6" s="33" t="s">
-        <v>46</v>
-      </c>
+      <c r="Q6" s="35"/>
       <c r="R6" s="34"/>
-      <c r="S6" s="33"/>
-      <c r="T6" s="33"/>
-      <c r="U6" s="35" t="n">
+      <c r="S6" s="34"/>
+      <c r="T6" s="36" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="V6" s="36" t="n">
+      <c r="U6" s="37" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="W6" s="36" t="n">
+      <c r="V6" s="37" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="X6" s="36" t="n">
+      <c r="W6" s="37" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Y6" s="36" t="n">
+      <c r="X6" s="37" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z6" s="37" t="n">
+      <c r="Y6" s="38" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AA6" s="38"/>
+      <c r="Z6" s="39"/>
+      <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="39" t="n">
+      <c r="B7" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="38"/>
+      <c r="C7" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="39"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="39"/>
-      <c r="L7" s="43"/>
-      <c r="M7" s="38"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="45"/>
       <c r="N7" s="44"/>
-      <c r="O7" s="43"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="44"/>
-      <c r="T7" s="45"/>
-      <c r="U7" s="46"/>
-      <c r="V7" s="47"/>
-      <c r="W7" s="47"/>
-      <c r="X7" s="47"/>
-      <c r="Y7" s="47"/>
-      <c r="Z7" s="48"/>
-      <c r="AA7" s="19"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="45"/>
+      <c r="S7" s="46"/>
+      <c r="T7" s="47"/>
+      <c r="U7" s="48"/>
+      <c r="V7" s="48"/>
+      <c r="W7" s="48"/>
+      <c r="X7" s="48"/>
+      <c r="Y7" s="49"/>
+      <c r="Z7" s="21"/>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="39" t="n">
+      <c r="B8" s="40" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="38"/>
+      <c r="C8" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="39"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="43"/>
-      <c r="M8" s="38"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="45"/>
       <c r="N8" s="44"/>
-      <c r="O8" s="43"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="44"/>
-      <c r="T8" s="45"/>
-      <c r="U8" s="46"/>
-      <c r="V8" s="47"/>
-      <c r="W8" s="47"/>
-      <c r="X8" s="47"/>
-      <c r="Y8" s="47"/>
-      <c r="Z8" s="48"/>
-      <c r="AA8" s="19"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="45"/>
+      <c r="S8" s="46"/>
+      <c r="T8" s="47"/>
+      <c r="U8" s="48"/>
+      <c r="V8" s="48"/>
+      <c r="W8" s="48"/>
+      <c r="X8" s="48"/>
+      <c r="Y8" s="49"/>
+      <c r="Z8" s="21"/>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="39" t="n">
+      <c r="B9" s="40" t="n">
         <v>3</v>
       </c>
-      <c r="C9" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="19"/>
+      <c r="C9" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="21"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="42"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="43"/>
-      <c r="M9" s="38"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="45"/>
       <c r="N9" s="44"/>
-      <c r="O9" s="43"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="44"/>
-      <c r="T9" s="45"/>
-      <c r="U9" s="46"/>
-      <c r="V9" s="47"/>
-      <c r="W9" s="47"/>
-      <c r="X9" s="47"/>
-      <c r="Y9" s="47"/>
-      <c r="Z9" s="48"/>
-      <c r="AA9" s="19"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="45"/>
+      <c r="S9" s="46"/>
+      <c r="T9" s="47"/>
+      <c r="U9" s="48"/>
+      <c r="V9" s="48"/>
+      <c r="W9" s="48"/>
+      <c r="X9" s="48"/>
+      <c r="Y9" s="49"/>
+      <c r="Z9" s="21"/>
     </row>
     <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="39" t="n">
+      <c r="B10" s="40" t="n">
         <v>4</v>
       </c>
-      <c r="C10" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="19"/>
+      <c r="C10" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="21"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="43"/>
-      <c r="M10" s="38"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="45"/>
       <c r="N10" s="44"/>
-      <c r="O10" s="43"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="44"/>
-      <c r="T10" s="45"/>
-      <c r="U10" s="46"/>
-      <c r="V10" s="47"/>
-      <c r="W10" s="47"/>
-      <c r="X10" s="47"/>
-      <c r="Y10" s="47"/>
-      <c r="Z10" s="48"/>
-      <c r="AA10" s="19"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="45"/>
+      <c r="S10" s="46"/>
+      <c r="T10" s="47"/>
+      <c r="U10" s="48"/>
+      <c r="V10" s="48"/>
+      <c r="W10" s="48"/>
+      <c r="X10" s="48"/>
+      <c r="Y10" s="49"/>
+      <c r="Z10" s="21"/>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="39" t="n">
+      <c r="B11" s="40" t="n">
         <v>5</v>
       </c>
-      <c r="C11" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="19"/>
+      <c r="C11" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="21"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="43"/>
-      <c r="M11" s="38"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="45"/>
       <c r="N11" s="44"/>
-      <c r="O11" s="43"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="44"/>
-      <c r="T11" s="45"/>
-      <c r="U11" s="46"/>
-      <c r="V11" s="47"/>
-      <c r="W11" s="47"/>
-      <c r="X11" s="47"/>
-      <c r="Y11" s="47"/>
-      <c r="Z11" s="48"/>
-      <c r="AA11" s="19"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="45"/>
+      <c r="S11" s="46"/>
+      <c r="T11" s="47"/>
+      <c r="U11" s="48"/>
+      <c r="V11" s="48"/>
+      <c r="W11" s="48"/>
+      <c r="X11" s="48"/>
+      <c r="Y11" s="49"/>
+      <c r="Z11" s="21"/>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="39" t="n">
+      <c r="B12" s="40" t="n">
         <v>6</v>
       </c>
-      <c r="C12" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="19"/>
+      <c r="C12" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="21"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="43"/>
-      <c r="M12" s="38"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="44"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="45"/>
       <c r="N12" s="44"/>
-      <c r="O12" s="43"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="44"/>
-      <c r="T12" s="45"/>
-      <c r="U12" s="46"/>
-      <c r="V12" s="47"/>
-      <c r="W12" s="47"/>
-      <c r="X12" s="47"/>
-      <c r="Y12" s="47"/>
-      <c r="Z12" s="48"/>
-      <c r="AA12" s="19"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="45"/>
+      <c r="S12" s="46"/>
+      <c r="T12" s="47"/>
+      <c r="U12" s="48"/>
+      <c r="V12" s="48"/>
+      <c r="W12" s="48"/>
+      <c r="X12" s="48"/>
+      <c r="Y12" s="49"/>
+      <c r="Z12" s="21"/>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="39" t="n">
+      <c r="B13" s="40" t="n">
         <v>7</v>
       </c>
-      <c r="C13" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="19"/>
+      <c r="C13" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="21"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="42"/>
-      <c r="K13" s="39"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="38"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="44"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="45"/>
       <c r="N13" s="44"/>
-      <c r="O13" s="43"/>
-      <c r="P13" s="19"/>
-      <c r="Q13" s="44"/>
-      <c r="T13" s="45"/>
-      <c r="U13" s="46"/>
-      <c r="V13" s="47"/>
-      <c r="W13" s="47"/>
-      <c r="X13" s="47"/>
-      <c r="Y13" s="47"/>
-      <c r="Z13" s="48"/>
-      <c r="AA13" s="19"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="45"/>
+      <c r="S13" s="46"/>
+      <c r="T13" s="47"/>
+      <c r="U13" s="48"/>
+      <c r="V13" s="48"/>
+      <c r="W13" s="48"/>
+      <c r="X13" s="48"/>
+      <c r="Y13" s="49"/>
+      <c r="Z13" s="21"/>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="39" t="n">
+      <c r="B14" s="40" t="n">
         <v>8</v>
       </c>
-      <c r="C14" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="19"/>
+      <c r="C14" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="21"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="43"/>
-      <c r="M14" s="38"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="44"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="45"/>
       <c r="N14" s="44"/>
-      <c r="O14" s="43"/>
-      <c r="P14" s="19"/>
-      <c r="Q14" s="44"/>
-      <c r="T14" s="45"/>
-      <c r="U14" s="46"/>
-      <c r="V14" s="47"/>
-      <c r="W14" s="47"/>
-      <c r="X14" s="47"/>
-      <c r="Y14" s="47"/>
-      <c r="Z14" s="48"/>
-      <c r="AA14" s="19"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="45"/>
+      <c r="S14" s="46"/>
+      <c r="T14" s="47"/>
+      <c r="U14" s="48"/>
+      <c r="V14" s="48"/>
+      <c r="W14" s="48"/>
+      <c r="X14" s="48"/>
+      <c r="Y14" s="49"/>
+      <c r="Z14" s="21"/>
     </row>
     <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="39" t="n">
+      <c r="B15" s="40" t="n">
         <v>9</v>
       </c>
-      <c r="C15" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="19"/>
+      <c r="C15" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="21"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="42"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="43"/>
-      <c r="M15" s="38"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="39"/>
+      <c r="M15" s="45"/>
       <c r="N15" s="44"/>
-      <c r="O15" s="43"/>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="44"/>
-      <c r="T15" s="45"/>
-      <c r="U15" s="46"/>
-      <c r="V15" s="47"/>
-      <c r="W15" s="47"/>
-      <c r="X15" s="47"/>
-      <c r="Y15" s="47"/>
-      <c r="Z15" s="48"/>
-      <c r="AA15" s="19"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="45"/>
+      <c r="S15" s="46"/>
+      <c r="T15" s="47"/>
+      <c r="U15" s="48"/>
+      <c r="V15" s="48"/>
+      <c r="W15" s="48"/>
+      <c r="X15" s="48"/>
+      <c r="Y15" s="49"/>
+      <c r="Z15" s="21"/>
     </row>
     <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="39" t="n">
+      <c r="B16" s="40" t="n">
         <v>10</v>
       </c>
-      <c r="C16" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="19"/>
+      <c r="C16" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="21"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="43"/>
-      <c r="M16" s="38"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="45"/>
       <c r="N16" s="44"/>
-      <c r="O16" s="43"/>
-      <c r="P16" s="19"/>
-      <c r="Q16" s="44"/>
-      <c r="T16" s="45"/>
-      <c r="U16" s="46"/>
-      <c r="V16" s="47"/>
-      <c r="W16" s="47"/>
-      <c r="X16" s="47"/>
-      <c r="Y16" s="47"/>
-      <c r="Z16" s="48"/>
-      <c r="AA16" s="19"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="45"/>
+      <c r="S16" s="46"/>
+      <c r="T16" s="47"/>
+      <c r="U16" s="48"/>
+      <c r="V16" s="48"/>
+      <c r="W16" s="48"/>
+      <c r="X16" s="48"/>
+      <c r="Y16" s="49"/>
+      <c r="Z16" s="21"/>
     </row>
     <row r="17" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="39" t="n">
+      <c r="B17" s="40" t="n">
         <v>11</v>
       </c>
-      <c r="C17" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="19"/>
+      <c r="C17" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="21"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="42"/>
-      <c r="K17" s="39"/>
-      <c r="L17" s="43"/>
-      <c r="M17" s="38"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="44"/>
+      <c r="L17" s="39"/>
+      <c r="M17" s="45"/>
       <c r="N17" s="44"/>
-      <c r="O17" s="43"/>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="44"/>
-      <c r="T17" s="45"/>
-      <c r="U17" s="46"/>
-      <c r="V17" s="47"/>
-      <c r="W17" s="47"/>
-      <c r="X17" s="47"/>
-      <c r="Y17" s="47"/>
-      <c r="Z17" s="48"/>
-      <c r="AA17" s="19"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="45"/>
+      <c r="S17" s="46"/>
+      <c r="T17" s="47"/>
+      <c r="U17" s="48"/>
+      <c r="V17" s="48"/>
+      <c r="W17" s="48"/>
+      <c r="X17" s="48"/>
+      <c r="Y17" s="49"/>
+      <c r="Z17" s="21"/>
     </row>
     <row r="18" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="39" t="n">
+      <c r="B18" s="40" t="n">
         <v>12</v>
       </c>
-      <c r="C18" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="19"/>
+      <c r="C18" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="21"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="43"/>
-      <c r="M18" s="38"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="44"/>
+      <c r="L18" s="39"/>
+      <c r="M18" s="45"/>
       <c r="N18" s="44"/>
-      <c r="O18" s="43"/>
-      <c r="P18" s="19"/>
-      <c r="Q18" s="44"/>
-      <c r="T18" s="45"/>
-      <c r="U18" s="46"/>
-      <c r="V18" s="47"/>
-      <c r="W18" s="47"/>
-      <c r="X18" s="47"/>
-      <c r="Y18" s="47"/>
-      <c r="Z18" s="48"/>
-      <c r="AA18" s="19"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="45"/>
+      <c r="S18" s="46"/>
+      <c r="T18" s="47"/>
+      <c r="U18" s="48"/>
+      <c r="V18" s="48"/>
+      <c r="W18" s="48"/>
+      <c r="X18" s="48"/>
+      <c r="Y18" s="49"/>
+      <c r="Z18" s="21"/>
     </row>
     <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="39" t="n">
+      <c r="B19" s="40" t="n">
         <v>13</v>
       </c>
-      <c r="C19" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="19"/>
+      <c r="C19" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="21"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="42"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="38"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="44"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="45"/>
       <c r="N19" s="44"/>
-      <c r="O19" s="43"/>
-      <c r="P19" s="19"/>
-      <c r="Q19" s="44"/>
-      <c r="T19" s="45"/>
-      <c r="U19" s="46"/>
-      <c r="V19" s="47"/>
-      <c r="W19" s="47"/>
-      <c r="X19" s="47"/>
-      <c r="Y19" s="47"/>
-      <c r="Z19" s="48"/>
-      <c r="AA19" s="19"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="45"/>
+      <c r="S19" s="46"/>
+      <c r="T19" s="47"/>
+      <c r="U19" s="48"/>
+      <c r="V19" s="48"/>
+      <c r="W19" s="48"/>
+      <c r="X19" s="48"/>
+      <c r="Y19" s="49"/>
+      <c r="Z19" s="21"/>
     </row>
     <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="39" t="n">
+      <c r="B20" s="40" t="n">
         <v>14</v>
       </c>
-      <c r="C20" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="19"/>
+      <c r="C20" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="21"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="43"/>
-      <c r="M20" s="38"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="44"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="45"/>
       <c r="N20" s="44"/>
-      <c r="O20" s="43"/>
-      <c r="P20" s="19"/>
-      <c r="Q20" s="44"/>
-      <c r="T20" s="45"/>
-      <c r="U20" s="46"/>
-      <c r="V20" s="47"/>
-      <c r="W20" s="47"/>
-      <c r="X20" s="47"/>
-      <c r="Y20" s="47"/>
-      <c r="Z20" s="48"/>
-      <c r="AA20" s="19"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="45"/>
+      <c r="S20" s="46"/>
+      <c r="T20" s="47"/>
+      <c r="U20" s="48"/>
+      <c r="V20" s="48"/>
+      <c r="W20" s="48"/>
+      <c r="X20" s="48"/>
+      <c r="Y20" s="49"/>
+      <c r="Z20" s="21"/>
     </row>
     <row r="21" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="39" t="n">
+      <c r="B21" s="40" t="n">
         <v>15</v>
       </c>
-      <c r="C21" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="19"/>
+      <c r="C21" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="21"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="43"/>
-      <c r="M21" s="38"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="44"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="45"/>
       <c r="N21" s="44"/>
-      <c r="O21" s="43"/>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="44"/>
-      <c r="T21" s="45"/>
-      <c r="U21" s="46"/>
-      <c r="V21" s="47"/>
-      <c r="W21" s="47"/>
-      <c r="X21" s="47"/>
-      <c r="Y21" s="47"/>
-      <c r="Z21" s="48"/>
-      <c r="AA21" s="19"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="45"/>
+      <c r="S21" s="46"/>
+      <c r="T21" s="47"/>
+      <c r="U21" s="48"/>
+      <c r="V21" s="48"/>
+      <c r="W21" s="48"/>
+      <c r="X21" s="48"/>
+      <c r="Y21" s="49"/>
+      <c r="Z21" s="21"/>
     </row>
     <row r="22" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="39" t="n">
+      <c r="B22" s="40" t="n">
         <v>16</v>
       </c>
-      <c r="C22" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="19"/>
+      <c r="C22" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="21"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="42"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="43"/>
-      <c r="M22" s="38"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="45"/>
       <c r="N22" s="44"/>
-      <c r="O22" s="43"/>
-      <c r="P22" s="19"/>
-      <c r="Q22" s="44"/>
-      <c r="T22" s="45"/>
-      <c r="U22" s="46"/>
-      <c r="V22" s="47"/>
-      <c r="W22" s="47"/>
-      <c r="X22" s="47"/>
-      <c r="Y22" s="47"/>
-      <c r="Z22" s="48"/>
-      <c r="AA22" s="19"/>
+      <c r="O22" s="21"/>
+      <c r="P22" s="45"/>
+      <c r="S22" s="46"/>
+      <c r="T22" s="47"/>
+      <c r="U22" s="48"/>
+      <c r="V22" s="48"/>
+      <c r="W22" s="48"/>
+      <c r="X22" s="48"/>
+      <c r="Y22" s="49"/>
+      <c r="Z22" s="21"/>
     </row>
     <row r="23" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="39" t="n">
+      <c r="B23" s="40" t="n">
         <v>17</v>
       </c>
-      <c r="C23" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" s="19"/>
+      <c r="C23" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="21"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="42"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="43"/>
-      <c r="M23" s="38"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="44"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="45"/>
       <c r="N23" s="44"/>
-      <c r="O23" s="43"/>
-      <c r="P23" s="19"/>
-      <c r="Q23" s="44"/>
-      <c r="T23" s="45"/>
-      <c r="U23" s="46"/>
-      <c r="V23" s="47"/>
-      <c r="W23" s="47"/>
-      <c r="X23" s="47"/>
-      <c r="Y23" s="47"/>
-      <c r="Z23" s="48"/>
-      <c r="AA23" s="19"/>
+      <c r="O23" s="21"/>
+      <c r="P23" s="45"/>
+      <c r="S23" s="46"/>
+      <c r="T23" s="47"/>
+      <c r="U23" s="48"/>
+      <c r="V23" s="48"/>
+      <c r="W23" s="48"/>
+      <c r="X23" s="48"/>
+      <c r="Y23" s="49"/>
+      <c r="Z23" s="21"/>
     </row>
     <row r="24" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="39" t="n">
+      <c r="B24" s="40" t="n">
         <v>18</v>
       </c>
-      <c r="C24" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" s="19"/>
+      <c r="C24" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="21"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="39"/>
-      <c r="L24" s="43"/>
-      <c r="M24" s="38"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="45"/>
       <c r="N24" s="44"/>
-      <c r="O24" s="43"/>
-      <c r="P24" s="19"/>
-      <c r="Q24" s="44"/>
-      <c r="T24" s="45"/>
-      <c r="U24" s="46"/>
-      <c r="V24" s="47"/>
-      <c r="W24" s="47"/>
-      <c r="X24" s="47"/>
-      <c r="Y24" s="47"/>
-      <c r="Z24" s="48"/>
-      <c r="AA24" s="19"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="45"/>
+      <c r="S24" s="46"/>
+      <c r="T24" s="47"/>
+      <c r="U24" s="48"/>
+      <c r="V24" s="48"/>
+      <c r="W24" s="48"/>
+      <c r="X24" s="48"/>
+      <c r="Y24" s="49"/>
+      <c r="Z24" s="21"/>
     </row>
     <row r="25" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="39" t="n">
+      <c r="B25" s="40" t="n">
         <v>19</v>
       </c>
-      <c r="C25" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" s="19"/>
+      <c r="C25" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="21"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="43"/>
-      <c r="M25" s="38"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="39"/>
+      <c r="M25" s="45"/>
       <c r="N25" s="44"/>
-      <c r="O25" s="43"/>
-      <c r="P25" s="19"/>
-      <c r="Q25" s="44"/>
-      <c r="T25" s="45"/>
-      <c r="U25" s="46"/>
-      <c r="V25" s="47"/>
-      <c r="W25" s="47"/>
-      <c r="X25" s="47"/>
-      <c r="Y25" s="47"/>
-      <c r="Z25" s="48"/>
-      <c r="AA25" s="19"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="45"/>
+      <c r="S25" s="46"/>
+      <c r="T25" s="47"/>
+      <c r="U25" s="48"/>
+      <c r="V25" s="48"/>
+      <c r="W25" s="48"/>
+      <c r="X25" s="48"/>
+      <c r="Y25" s="49"/>
+      <c r="Z25" s="21"/>
     </row>
     <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="39" t="n">
+      <c r="B26" s="40" t="n">
         <v>20</v>
       </c>
-      <c r="C26" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="19"/>
+      <c r="C26" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="21"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
-      <c r="H26" s="41"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="43"/>
-      <c r="M26" s="38"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="39"/>
+      <c r="M26" s="45"/>
       <c r="N26" s="44"/>
-      <c r="O26" s="43"/>
-      <c r="P26" s="19"/>
-      <c r="Q26" s="44"/>
-      <c r="T26" s="45"/>
-      <c r="U26" s="46"/>
-      <c r="V26" s="47"/>
-      <c r="W26" s="47"/>
-      <c r="X26" s="47"/>
-      <c r="Y26" s="47"/>
-      <c r="Z26" s="48"/>
-      <c r="AA26" s="19"/>
+      <c r="O26" s="21"/>
+      <c r="P26" s="45"/>
+      <c r="S26" s="46"/>
+      <c r="T26" s="47"/>
+      <c r="U26" s="48"/>
+      <c r="V26" s="48"/>
+      <c r="W26" s="48"/>
+      <c r="X26" s="48"/>
+      <c r="Y26" s="49"/>
+      <c r="Z26" s="21"/>
     </row>
     <row r="27" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="39" t="n">
+      <c r="B27" s="40" t="n">
         <v>21</v>
       </c>
-      <c r="C27" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" s="19"/>
+      <c r="C27" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="21"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
-      <c r="H27" s="41"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="42"/>
-      <c r="K27" s="39"/>
-      <c r="L27" s="43"/>
-      <c r="M27" s="38"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="44"/>
+      <c r="L27" s="39"/>
+      <c r="M27" s="45"/>
       <c r="N27" s="44"/>
-      <c r="O27" s="43"/>
-      <c r="P27" s="19"/>
-      <c r="Q27" s="44"/>
-      <c r="T27" s="45"/>
-      <c r="U27" s="46"/>
-      <c r="V27" s="47"/>
-      <c r="W27" s="47"/>
-      <c r="X27" s="47"/>
-      <c r="Y27" s="47"/>
-      <c r="Z27" s="48"/>
-      <c r="AA27" s="19"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="45"/>
+      <c r="S27" s="46"/>
+      <c r="T27" s="47"/>
+      <c r="U27" s="48"/>
+      <c r="V27" s="48"/>
+      <c r="W27" s="48"/>
+      <c r="X27" s="48"/>
+      <c r="Y27" s="49"/>
+      <c r="Z27" s="21"/>
     </row>
     <row r="28" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="39" t="n">
+      <c r="B28" s="40" t="n">
         <v>22</v>
       </c>
-      <c r="C28" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D28" s="19"/>
+      <c r="C28" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="21"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="42"/>
-      <c r="K28" s="39"/>
-      <c r="L28" s="43"/>
-      <c r="M28" s="38"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="40"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="39"/>
+      <c r="M28" s="45"/>
       <c r="N28" s="44"/>
-      <c r="O28" s="43"/>
-      <c r="P28" s="19"/>
-      <c r="Q28" s="44"/>
-      <c r="T28" s="45"/>
-      <c r="U28" s="46"/>
-      <c r="V28" s="47"/>
-      <c r="W28" s="47"/>
-      <c r="X28" s="47"/>
-      <c r="Y28" s="47"/>
-      <c r="Z28" s="48"/>
-      <c r="AA28" s="19"/>
+      <c r="O28" s="21"/>
+      <c r="P28" s="45"/>
+      <c r="S28" s="46"/>
+      <c r="T28" s="47"/>
+      <c r="U28" s="48"/>
+      <c r="V28" s="48"/>
+      <c r="W28" s="48"/>
+      <c r="X28" s="48"/>
+      <c r="Y28" s="49"/>
+      <c r="Z28" s="21"/>
     </row>
     <row r="29" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="39" t="n">
+      <c r="B29" s="40" t="n">
         <v>23</v>
       </c>
-      <c r="C29" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29" s="19"/>
+      <c r="C29" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="21"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
-      <c r="H29" s="41"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="42"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="43"/>
-      <c r="M29" s="19"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="40"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="45"/>
       <c r="N29" s="44"/>
-      <c r="O29" s="43"/>
-      <c r="P29" s="19"/>
-      <c r="Q29" s="44"/>
-      <c r="T29" s="45"/>
-      <c r="U29" s="46"/>
-      <c r="V29" s="47"/>
-      <c r="W29" s="47"/>
-      <c r="X29" s="47"/>
-      <c r="Y29" s="47"/>
-      <c r="Z29" s="48"/>
-      <c r="AA29" s="19"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="45"/>
+      <c r="S29" s="46"/>
+      <c r="T29" s="47"/>
+      <c r="U29" s="48"/>
+      <c r="V29" s="48"/>
+      <c r="W29" s="48"/>
+      <c r="X29" s="48"/>
+      <c r="Y29" s="49"/>
+      <c r="Z29" s="21"/>
     </row>
     <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="39" t="n">
+      <c r="B30" s="40" t="n">
         <v>24</v>
       </c>
-      <c r="C30" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D30" s="19"/>
+      <c r="C30" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="21"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="42"/>
-      <c r="K30" s="39"/>
-      <c r="L30" s="43"/>
-      <c r="M30" s="19"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="43"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="44"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="45"/>
       <c r="N30" s="44"/>
-      <c r="O30" s="43"/>
-      <c r="P30" s="19"/>
-      <c r="Q30" s="44"/>
-      <c r="T30" s="45"/>
-      <c r="U30" s="46"/>
-      <c r="V30" s="47"/>
-      <c r="W30" s="47"/>
-      <c r="X30" s="47"/>
-      <c r="Y30" s="47"/>
-      <c r="Z30" s="48"/>
-      <c r="AA30" s="19"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="45"/>
+      <c r="S30" s="46"/>
+      <c r="T30" s="47"/>
+      <c r="U30" s="48"/>
+      <c r="V30" s="48"/>
+      <c r="W30" s="48"/>
+      <c r="X30" s="48"/>
+      <c r="Y30" s="49"/>
+      <c r="Z30" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:Z1"/>
+    <mergeCell ref="E1:Y1"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="U4:Z4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="T4:Y4"/>
   </mergeCells>
-  <dataValidations count="14">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="U6:Z30" type="list">
+  <dataValidations count="13">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T6:Y30" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J30" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I30" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K30" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J30" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1958,7 +1959,7 @@
       <formula1>"transmission,fluorescence,both,reference,yield,test"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I30" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6:H30" type="list">
       <formula1>"Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1974,27 +1975,23 @@
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6:H30" type="decimal">
-      <formula1>4500</formula1>
-      <formula2>23500</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T7:T30" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S7:S30" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T6" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:S30" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:R30" type="decimal">
       <formula1>10</formula1>
       <formula2>400</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R7:R30" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Q7:Q30" type="decimal">
       <formula1>-150</formula1>
       <formula2>150</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Q6" type="decimal">
       <formula1>-150</formula1>
       <formula2>150</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
more work on wheel, reinstate M1 T monitoring
</commit_message>
<xml_diff>
--- a/startup/wheel_template.xlsx
+++ b/startup/wheel_template.xlsx
@@ -708,9 +708,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1227600</xdr:colOff>
+      <xdr:colOff>1227240</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>61200</xdr:rowOff>
+      <xdr:rowOff>60840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -724,7 +724,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="6933960"/>
-          <a:ext cx="2518560" cy="2744280"/>
+          <a:ext cx="2517840" cy="2743920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -744,10 +744,10 @@
       <xdr:rowOff>106560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>919080</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>826200</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>129960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -756,8 +756,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3190320" y="6959880"/>
-          <a:ext cx="4648320" cy="1645560"/>
+          <a:off x="3189600" y="6959880"/>
+          <a:ext cx="6645240" cy="1811520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -891,7 +891,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>5. Specify motor/slit positions in columns R,S,T; leave blank for no motion </a:t>
+            <a:t>5. Specify motor/slit positions in columns Q,R,S; leave blank for no motion </a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -929,7 +929,26 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>7. Do not add columns before column Z</a:t>
+            <a:t>7. Do not add columns before column Y</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>8. The wheel is correctly mounted if the numbers can be read when facing the wheel</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -950,10 +969,10 @@
   <dimension ref="B1:AMJ30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="6" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="6" topLeftCell="E31" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="bottomLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
       <selection pane="bottomRight" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -963,12 +982,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="0" width="29.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="14" style="0" width="22.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="17" style="0" width="14.43"/>

</xml_diff>

<commit_message>
flags in wheel spreadsheet
</commit_message>
<xml_diff>
--- a/startup/wheel_template.xlsx
+++ b/startup/wheel_template.xlsx
@@ -20,11 +20,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
   <si>
     <t xml:space="preserve">Experimenters:</t>
   </si>
   <si>
+    <t xml:space="preserve">Change edge at start?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Close shutter at end?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
     <t xml:space="preserve">File name</t>
   </si>
   <si>
@@ -119,9 +131,6 @@
   </si>
   <si>
     <t xml:space="preserve">Default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
   </si>
   <si>
     <t xml:space="preserve">best_sample_ever</t>
@@ -219,7 +228,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -234,17 +243,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFDBB6"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFCCCCCC"/>
         <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -424,7 +453,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -445,27 +474,35 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -473,7 +510,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -481,7 +518,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -489,15 +526,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -513,26 +550,18 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -542,6 +571,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -549,15 +590,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -565,11 +598,15 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -577,7 +614,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -585,15 +622,15 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -601,19 +638,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -621,7 +658,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -675,7 +712,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFDBB6"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -708,9 +745,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1227240</xdr:colOff>
+      <xdr:colOff>1226880</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>60840</xdr:rowOff>
+      <xdr:rowOff>60480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -724,7 +761,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="6933960"/>
-          <a:ext cx="2517840" cy="2743920"/>
+          <a:ext cx="2517480" cy="2743560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -745,9 +782,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>826200</xdr:colOff>
+      <xdr:colOff>825840</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>129960</xdr:rowOff>
+      <xdr:rowOff>129600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -757,7 +794,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3189600" y="6959880"/>
-          <a:ext cx="6645240" cy="1811520"/>
+          <a:ext cx="6644880" cy="1811160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -969,30 +1006,27 @@
   <dimension ref="B1:AMJ30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="6" topLeftCell="E31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
-      <selection pane="bottomRight" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="0" width="29.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="14" style="0" width="22.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="17" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="25" min="20" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="26" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="25" min="20" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1025,934 +1059,947 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="H2" s="1"/>
+      <c r="E2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="5"/>
+      <c r="J2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="8"/>
       <c r="U2" s="0"/>
       <c r="V2" s="0"/>
       <c r="W2" s="0"/>
       <c r="X2" s="0"/>
-      <c r="Y2" s="5"/>
+      <c r="Y2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="5"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="8"/>
       <c r="U3" s="0"/>
       <c r="V3" s="0"/>
       <c r="W3" s="0"/>
       <c r="X3" s="0"/>
-      <c r="Y3" s="5"/>
+      <c r="Y3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="12"/>
+    </row>
+    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="P5" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q5" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="R5" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="S5" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="T5" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="U5" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="V5" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="W5" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="X5" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y5" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z5" s="22"/>
+    </row>
+    <row r="6" s="23" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B6" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-    </row>
-    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="N5" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="O5" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="P5" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q5" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="R5" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="S5" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="T5" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="U5" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="V5" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="W5" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="X5" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y5" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z5" s="20"/>
-    </row>
-    <row r="6" s="21" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" s="27" t="s">
+      <c r="F6" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="28" t="s">
+      <c r="G6" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="K6" s="29" t="s">
+      <c r="H6" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="30" t="s">
+      <c r="I6" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="M6" s="31" t="s">
+      <c r="J6" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="N6" s="32" t="s">
+      <c r="K6" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="O6" s="33" t="s">
+      <c r="L6" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="P6" s="34" t="s">
+      <c r="M6" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="Q6" s="35"/>
-      <c r="R6" s="34"/>
-      <c r="S6" s="34"/>
-      <c r="T6" s="36" t="n">
+      <c r="N6" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="O6" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="P6" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="36"/>
+      <c r="S6" s="36"/>
+      <c r="T6" s="38" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U6" s="37" t="n">
+      <c r="U6" s="39" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="V6" s="37" t="n">
+      <c r="V6" s="39" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="W6" s="37" t="n">
+      <c r="W6" s="39" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="X6" s="37" t="n">
+      <c r="X6" s="39" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Y6" s="38" t="n">
+      <c r="Y6" s="40" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z6" s="39"/>
+      <c r="Z6" s="41"/>
       <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="40" t="n">
+      <c r="B7" s="42" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="39"/>
+      <c r="C7" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="41"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="44"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="45"/>
-      <c r="N7" s="44"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="45"/>
-      <c r="S7" s="46"/>
-      <c r="T7" s="47"/>
-      <c r="U7" s="48"/>
-      <c r="V7" s="48"/>
-      <c r="W7" s="48"/>
-      <c r="X7" s="48"/>
-      <c r="Y7" s="49"/>
-      <c r="Z7" s="21"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="46"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="47"/>
+      <c r="S7" s="48"/>
+      <c r="T7" s="49"/>
+      <c r="U7" s="50"/>
+      <c r="V7" s="50"/>
+      <c r="W7" s="50"/>
+      <c r="X7" s="50"/>
+      <c r="Y7" s="51"/>
+      <c r="Z7" s="23"/>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="40" t="n">
+      <c r="B8" s="42" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="39"/>
+      <c r="C8" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="41"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="45"/>
-      <c r="N8" s="44"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="45"/>
-      <c r="S8" s="46"/>
-      <c r="T8" s="47"/>
-      <c r="U8" s="48"/>
-      <c r="V8" s="48"/>
-      <c r="W8" s="48"/>
-      <c r="X8" s="48"/>
-      <c r="Y8" s="49"/>
-      <c r="Z8" s="21"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="46"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="47"/>
+      <c r="S8" s="48"/>
+      <c r="T8" s="49"/>
+      <c r="U8" s="50"/>
+      <c r="V8" s="50"/>
+      <c r="W8" s="50"/>
+      <c r="X8" s="50"/>
+      <c r="Y8" s="51"/>
+      <c r="Z8" s="23"/>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="40" t="n">
+      <c r="B9" s="42" t="n">
         <v>3</v>
       </c>
-      <c r="C9" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="21"/>
+      <c r="C9" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="23"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="45"/>
-      <c r="N9" s="44"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="45"/>
-      <c r="S9" s="46"/>
-      <c r="T9" s="47"/>
-      <c r="U9" s="48"/>
-      <c r="V9" s="48"/>
-      <c r="W9" s="48"/>
-      <c r="X9" s="48"/>
-      <c r="Y9" s="49"/>
-      <c r="Z9" s="21"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="46"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="47"/>
+      <c r="S9" s="48"/>
+      <c r="T9" s="49"/>
+      <c r="U9" s="50"/>
+      <c r="V9" s="50"/>
+      <c r="W9" s="50"/>
+      <c r="X9" s="50"/>
+      <c r="Y9" s="51"/>
+      <c r="Z9" s="23"/>
     </row>
     <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="40" t="n">
-        <v>4</v>
-      </c>
-      <c r="C10" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="21"/>
+      <c r="B10" s="42" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="23"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="45"/>
-      <c r="N10" s="44"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="45"/>
-      <c r="S10" s="46"/>
-      <c r="T10" s="47"/>
-      <c r="U10" s="48"/>
-      <c r="V10" s="48"/>
-      <c r="W10" s="48"/>
-      <c r="X10" s="48"/>
-      <c r="Y10" s="49"/>
-      <c r="Z10" s="21"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="46"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="47"/>
+      <c r="S10" s="48"/>
+      <c r="T10" s="49"/>
+      <c r="U10" s="50"/>
+      <c r="V10" s="50"/>
+      <c r="W10" s="50"/>
+      <c r="X10" s="50"/>
+      <c r="Y10" s="51"/>
+      <c r="Z10" s="23"/>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="40" t="n">
+      <c r="B11" s="42" t="n">
         <v>5</v>
       </c>
-      <c r="C11" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="21"/>
+      <c r="C11" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="23"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="45"/>
-      <c r="N11" s="44"/>
-      <c r="O11" s="21"/>
-      <c r="P11" s="45"/>
-      <c r="S11" s="46"/>
-      <c r="T11" s="47"/>
-      <c r="U11" s="48"/>
-      <c r="V11" s="48"/>
-      <c r="W11" s="48"/>
-      <c r="X11" s="48"/>
-      <c r="Y11" s="49"/>
-      <c r="Z11" s="21"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="46"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="47"/>
+      <c r="S11" s="48"/>
+      <c r="T11" s="49"/>
+      <c r="U11" s="50"/>
+      <c r="V11" s="50"/>
+      <c r="W11" s="50"/>
+      <c r="X11" s="50"/>
+      <c r="Y11" s="51"/>
+      <c r="Z11" s="23"/>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="40" t="n">
+      <c r="B12" s="42" t="n">
         <v>6</v>
       </c>
-      <c r="C12" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="21"/>
+      <c r="C12" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="23"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="44"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="44"/>
-      <c r="O12" s="21"/>
-      <c r="P12" s="45"/>
-      <c r="S12" s="46"/>
-      <c r="T12" s="47"/>
-      <c r="U12" s="48"/>
-      <c r="V12" s="48"/>
-      <c r="W12" s="48"/>
-      <c r="X12" s="48"/>
-      <c r="Y12" s="49"/>
-      <c r="Z12" s="21"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="46"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="46"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="47"/>
+      <c r="S12" s="48"/>
+      <c r="T12" s="49"/>
+      <c r="U12" s="50"/>
+      <c r="V12" s="50"/>
+      <c r="W12" s="50"/>
+      <c r="X12" s="50"/>
+      <c r="Y12" s="51"/>
+      <c r="Z12" s="23"/>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="40" t="n">
+      <c r="B13" s="42" t="n">
         <v>7</v>
       </c>
-      <c r="C13" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="21"/>
+      <c r="C13" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="23"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="44"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="45"/>
-      <c r="N13" s="44"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="45"/>
-      <c r="S13" s="46"/>
-      <c r="T13" s="47"/>
-      <c r="U13" s="48"/>
-      <c r="V13" s="48"/>
-      <c r="W13" s="48"/>
-      <c r="X13" s="48"/>
-      <c r="Y13" s="49"/>
-      <c r="Z13" s="21"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="46"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="47"/>
+      <c r="N13" s="46"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="47"/>
+      <c r="S13" s="48"/>
+      <c r="T13" s="49"/>
+      <c r="U13" s="50"/>
+      <c r="V13" s="50"/>
+      <c r="W13" s="50"/>
+      <c r="X13" s="50"/>
+      <c r="Y13" s="51"/>
+      <c r="Z13" s="23"/>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="40" t="n">
+      <c r="B14" s="42" t="n">
         <v>8</v>
       </c>
-      <c r="C14" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="21"/>
+      <c r="C14" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="23"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="44"/>
-      <c r="L14" s="39"/>
-      <c r="M14" s="45"/>
-      <c r="N14" s="44"/>
-      <c r="O14" s="21"/>
-      <c r="P14" s="45"/>
-      <c r="S14" s="46"/>
-      <c r="T14" s="47"/>
-      <c r="U14" s="48"/>
-      <c r="V14" s="48"/>
-      <c r="W14" s="48"/>
-      <c r="X14" s="48"/>
-      <c r="Y14" s="49"/>
-      <c r="Z14" s="21"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="46"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="47"/>
+      <c r="N14" s="46"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="47"/>
+      <c r="S14" s="48"/>
+      <c r="T14" s="49"/>
+      <c r="U14" s="50"/>
+      <c r="V14" s="50"/>
+      <c r="W14" s="50"/>
+      <c r="X14" s="50"/>
+      <c r="Y14" s="51"/>
+      <c r="Z14" s="23"/>
     </row>
     <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="40" t="n">
+      <c r="B15" s="42" t="n">
         <v>9</v>
       </c>
-      <c r="C15" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="21"/>
+      <c r="C15" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="23"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="43"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="44"/>
-      <c r="L15" s="39"/>
-      <c r="M15" s="45"/>
-      <c r="N15" s="44"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="45"/>
-      <c r="S15" s="46"/>
-      <c r="T15" s="47"/>
-      <c r="U15" s="48"/>
-      <c r="V15" s="48"/>
-      <c r="W15" s="48"/>
-      <c r="X15" s="48"/>
-      <c r="Y15" s="49"/>
-      <c r="Z15" s="21"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="46"/>
+      <c r="L15" s="41"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="46"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="47"/>
+      <c r="S15" s="48"/>
+      <c r="T15" s="49"/>
+      <c r="U15" s="50"/>
+      <c r="V15" s="50"/>
+      <c r="W15" s="50"/>
+      <c r="X15" s="50"/>
+      <c r="Y15" s="51"/>
+      <c r="Z15" s="23"/>
     </row>
     <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="40" t="n">
+      <c r="B16" s="42" t="n">
         <v>10</v>
       </c>
-      <c r="C16" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="21"/>
+      <c r="C16" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="23"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="43"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="44"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="45"/>
-      <c r="N16" s="44"/>
-      <c r="O16" s="21"/>
-      <c r="P16" s="45"/>
-      <c r="S16" s="46"/>
-      <c r="T16" s="47"/>
-      <c r="U16" s="48"/>
-      <c r="V16" s="48"/>
-      <c r="W16" s="48"/>
-      <c r="X16" s="48"/>
-      <c r="Y16" s="49"/>
-      <c r="Z16" s="21"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="46"/>
+      <c r="L16" s="41"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="46"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="47"/>
+      <c r="S16" s="48"/>
+      <c r="T16" s="49"/>
+      <c r="U16" s="50"/>
+      <c r="V16" s="50"/>
+      <c r="W16" s="50"/>
+      <c r="X16" s="50"/>
+      <c r="Y16" s="51"/>
+      <c r="Z16" s="23"/>
     </row>
     <row r="17" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="40" t="n">
+      <c r="B17" s="42" t="n">
         <v>11</v>
       </c>
-      <c r="C17" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="21"/>
+      <c r="C17" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="23"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="44"/>
-      <c r="L17" s="39"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="44"/>
-      <c r="O17" s="21"/>
-      <c r="P17" s="45"/>
-      <c r="S17" s="46"/>
-      <c r="T17" s="47"/>
-      <c r="U17" s="48"/>
-      <c r="V17" s="48"/>
-      <c r="W17" s="48"/>
-      <c r="X17" s="48"/>
-      <c r="Y17" s="49"/>
-      <c r="Z17" s="21"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="41"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="46"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="47"/>
+      <c r="S17" s="48"/>
+      <c r="T17" s="49"/>
+      <c r="U17" s="50"/>
+      <c r="V17" s="50"/>
+      <c r="W17" s="50"/>
+      <c r="X17" s="50"/>
+      <c r="Y17" s="51"/>
+      <c r="Z17" s="23"/>
     </row>
     <row r="18" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="40" t="n">
+      <c r="B18" s="42" t="n">
         <v>12</v>
       </c>
-      <c r="C18" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="21"/>
+      <c r="C18" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="23"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="44"/>
-      <c r="L18" s="39"/>
-      <c r="M18" s="45"/>
-      <c r="N18" s="44"/>
-      <c r="O18" s="21"/>
-      <c r="P18" s="45"/>
-      <c r="S18" s="46"/>
-      <c r="T18" s="47"/>
-      <c r="U18" s="48"/>
-      <c r="V18" s="48"/>
-      <c r="W18" s="48"/>
-      <c r="X18" s="48"/>
-      <c r="Y18" s="49"/>
-      <c r="Z18" s="21"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="41"/>
+      <c r="M18" s="47"/>
+      <c r="N18" s="46"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="47"/>
+      <c r="S18" s="48"/>
+      <c r="T18" s="49"/>
+      <c r="U18" s="50"/>
+      <c r="V18" s="50"/>
+      <c r="W18" s="50"/>
+      <c r="X18" s="50"/>
+      <c r="Y18" s="51"/>
+      <c r="Z18" s="23"/>
     </row>
     <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="40" t="n">
+      <c r="B19" s="42" t="n">
         <v>13</v>
       </c>
-      <c r="C19" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="21"/>
+      <c r="C19" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="23"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="44"/>
-      <c r="L19" s="39"/>
-      <c r="M19" s="45"/>
-      <c r="N19" s="44"/>
-      <c r="O19" s="21"/>
-      <c r="P19" s="45"/>
-      <c r="S19" s="46"/>
-      <c r="T19" s="47"/>
-      <c r="U19" s="48"/>
-      <c r="V19" s="48"/>
-      <c r="W19" s="48"/>
-      <c r="X19" s="48"/>
-      <c r="Y19" s="49"/>
-      <c r="Z19" s="21"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="46"/>
+      <c r="L19" s="41"/>
+      <c r="M19" s="47"/>
+      <c r="N19" s="46"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="47"/>
+      <c r="S19" s="48"/>
+      <c r="T19" s="49"/>
+      <c r="U19" s="50"/>
+      <c r="V19" s="50"/>
+      <c r="W19" s="50"/>
+      <c r="X19" s="50"/>
+      <c r="Y19" s="51"/>
+      <c r="Z19" s="23"/>
     </row>
     <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="40" t="n">
+      <c r="B20" s="42" t="n">
         <v>14</v>
       </c>
-      <c r="C20" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="21"/>
+      <c r="C20" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="23"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="44"/>
-      <c r="L20" s="39"/>
-      <c r="M20" s="45"/>
-      <c r="N20" s="44"/>
-      <c r="O20" s="21"/>
-      <c r="P20" s="45"/>
-      <c r="S20" s="46"/>
-      <c r="T20" s="47"/>
-      <c r="U20" s="48"/>
-      <c r="V20" s="48"/>
-      <c r="W20" s="48"/>
-      <c r="X20" s="48"/>
-      <c r="Y20" s="49"/>
-      <c r="Z20" s="21"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="46"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="47"/>
+      <c r="N20" s="46"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="47"/>
+      <c r="S20" s="48"/>
+      <c r="T20" s="49"/>
+      <c r="U20" s="50"/>
+      <c r="V20" s="50"/>
+      <c r="W20" s="50"/>
+      <c r="X20" s="50"/>
+      <c r="Y20" s="51"/>
+      <c r="Z20" s="23"/>
     </row>
     <row r="21" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="40" t="n">
+      <c r="B21" s="42" t="n">
         <v>15</v>
       </c>
-      <c r="C21" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="21"/>
+      <c r="C21" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="23"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="40"/>
-      <c r="K21" s="44"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="45"/>
-      <c r="N21" s="44"/>
-      <c r="O21" s="21"/>
-      <c r="P21" s="45"/>
-      <c r="S21" s="46"/>
-      <c r="T21" s="47"/>
-      <c r="U21" s="48"/>
-      <c r="V21" s="48"/>
-      <c r="W21" s="48"/>
-      <c r="X21" s="48"/>
-      <c r="Y21" s="49"/>
-      <c r="Z21" s="21"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="41"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="46"/>
+      <c r="O21" s="23"/>
+      <c r="P21" s="47"/>
+      <c r="S21" s="48"/>
+      <c r="T21" s="49"/>
+      <c r="U21" s="50"/>
+      <c r="V21" s="50"/>
+      <c r="W21" s="50"/>
+      <c r="X21" s="50"/>
+      <c r="Y21" s="51"/>
+      <c r="Z21" s="23"/>
     </row>
     <row r="22" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="40" t="n">
+      <c r="B22" s="42" t="n">
         <v>16</v>
       </c>
-      <c r="C22" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="21"/>
+      <c r="C22" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="23"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="40"/>
-      <c r="K22" s="44"/>
-      <c r="L22" s="39"/>
-      <c r="M22" s="45"/>
-      <c r="N22" s="44"/>
-      <c r="O22" s="21"/>
-      <c r="P22" s="45"/>
-      <c r="S22" s="46"/>
-      <c r="T22" s="47"/>
-      <c r="U22" s="48"/>
-      <c r="V22" s="48"/>
-      <c r="W22" s="48"/>
-      <c r="X22" s="48"/>
-      <c r="Y22" s="49"/>
-      <c r="Z22" s="21"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="41"/>
+      <c r="M22" s="47"/>
+      <c r="N22" s="46"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="47"/>
+      <c r="S22" s="48"/>
+      <c r="T22" s="49"/>
+      <c r="U22" s="50"/>
+      <c r="V22" s="50"/>
+      <c r="W22" s="50"/>
+      <c r="X22" s="50"/>
+      <c r="Y22" s="51"/>
+      <c r="Z22" s="23"/>
     </row>
     <row r="23" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="40" t="n">
+      <c r="B23" s="42" t="n">
         <v>17</v>
       </c>
-      <c r="C23" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="21"/>
+      <c r="C23" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="23"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="40"/>
-      <c r="K23" s="44"/>
-      <c r="L23" s="39"/>
-      <c r="M23" s="45"/>
-      <c r="N23" s="44"/>
-      <c r="O23" s="21"/>
-      <c r="P23" s="45"/>
-      <c r="S23" s="46"/>
-      <c r="T23" s="47"/>
-      <c r="U23" s="48"/>
-      <c r="V23" s="48"/>
-      <c r="W23" s="48"/>
-      <c r="X23" s="48"/>
-      <c r="Y23" s="49"/>
-      <c r="Z23" s="21"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="46"/>
+      <c r="L23" s="41"/>
+      <c r="M23" s="47"/>
+      <c r="N23" s="46"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="47"/>
+      <c r="S23" s="48"/>
+      <c r="T23" s="49"/>
+      <c r="U23" s="50"/>
+      <c r="V23" s="50"/>
+      <c r="W23" s="50"/>
+      <c r="X23" s="50"/>
+      <c r="Y23" s="51"/>
+      <c r="Z23" s="23"/>
     </row>
     <row r="24" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="40" t="n">
+      <c r="B24" s="42" t="n">
         <v>18</v>
       </c>
-      <c r="C24" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="21"/>
+      <c r="C24" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="23"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="40"/>
-      <c r="K24" s="44"/>
-      <c r="L24" s="39"/>
-      <c r="M24" s="45"/>
-      <c r="N24" s="44"/>
-      <c r="O24" s="21"/>
-      <c r="P24" s="45"/>
-      <c r="S24" s="46"/>
-      <c r="T24" s="47"/>
-      <c r="U24" s="48"/>
-      <c r="V24" s="48"/>
-      <c r="W24" s="48"/>
-      <c r="X24" s="48"/>
-      <c r="Y24" s="49"/>
-      <c r="Z24" s="21"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="41"/>
+      <c r="M24" s="47"/>
+      <c r="N24" s="46"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="47"/>
+      <c r="S24" s="48"/>
+      <c r="T24" s="49"/>
+      <c r="U24" s="50"/>
+      <c r="V24" s="50"/>
+      <c r="W24" s="50"/>
+      <c r="X24" s="50"/>
+      <c r="Y24" s="51"/>
+      <c r="Z24" s="23"/>
     </row>
     <row r="25" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="40" t="n">
+      <c r="B25" s="42" t="n">
         <v>19</v>
       </c>
-      <c r="C25" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="21"/>
+      <c r="C25" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="23"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="43"/>
-      <c r="J25" s="40"/>
-      <c r="K25" s="44"/>
-      <c r="L25" s="39"/>
-      <c r="M25" s="45"/>
-      <c r="N25" s="44"/>
-      <c r="O25" s="21"/>
-      <c r="P25" s="45"/>
-      <c r="S25" s="46"/>
-      <c r="T25" s="47"/>
-      <c r="U25" s="48"/>
-      <c r="V25" s="48"/>
-      <c r="W25" s="48"/>
-      <c r="X25" s="48"/>
-      <c r="Y25" s="49"/>
-      <c r="Z25" s="21"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="41"/>
+      <c r="M25" s="47"/>
+      <c r="N25" s="46"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="47"/>
+      <c r="S25" s="48"/>
+      <c r="T25" s="49"/>
+      <c r="U25" s="50"/>
+      <c r="V25" s="50"/>
+      <c r="W25" s="50"/>
+      <c r="X25" s="50"/>
+      <c r="Y25" s="51"/>
+      <c r="Z25" s="23"/>
     </row>
     <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="40" t="n">
+      <c r="B26" s="42" t="n">
         <v>20</v>
       </c>
-      <c r="C26" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="21"/>
+      <c r="C26" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="23"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="40"/>
-      <c r="K26" s="44"/>
-      <c r="L26" s="39"/>
-      <c r="M26" s="45"/>
-      <c r="N26" s="44"/>
-      <c r="O26" s="21"/>
-      <c r="P26" s="45"/>
-      <c r="S26" s="46"/>
-      <c r="T26" s="47"/>
-      <c r="U26" s="48"/>
-      <c r="V26" s="48"/>
-      <c r="W26" s="48"/>
-      <c r="X26" s="48"/>
-      <c r="Y26" s="49"/>
-      <c r="Z26" s="21"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="45"/>
+      <c r="J26" s="42"/>
+      <c r="K26" s="46"/>
+      <c r="L26" s="41"/>
+      <c r="M26" s="47"/>
+      <c r="N26" s="46"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="47"/>
+      <c r="S26" s="48"/>
+      <c r="T26" s="49"/>
+      <c r="U26" s="50"/>
+      <c r="V26" s="50"/>
+      <c r="W26" s="50"/>
+      <c r="X26" s="50"/>
+      <c r="Y26" s="51"/>
+      <c r="Z26" s="23"/>
     </row>
     <row r="27" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="40" t="n">
+      <c r="B27" s="42" t="n">
         <v>21</v>
       </c>
-      <c r="C27" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="21"/>
+      <c r="C27" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="23"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="40"/>
-      <c r="K27" s="44"/>
-      <c r="L27" s="39"/>
-      <c r="M27" s="45"/>
-      <c r="N27" s="44"/>
-      <c r="O27" s="21"/>
-      <c r="P27" s="45"/>
-      <c r="S27" s="46"/>
-      <c r="T27" s="47"/>
-      <c r="U27" s="48"/>
-      <c r="V27" s="48"/>
-      <c r="W27" s="48"/>
-      <c r="X27" s="48"/>
-      <c r="Y27" s="49"/>
-      <c r="Z27" s="21"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="42"/>
+      <c r="K27" s="46"/>
+      <c r="L27" s="41"/>
+      <c r="M27" s="47"/>
+      <c r="N27" s="46"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="47"/>
+      <c r="S27" s="48"/>
+      <c r="T27" s="49"/>
+      <c r="U27" s="50"/>
+      <c r="V27" s="50"/>
+      <c r="W27" s="50"/>
+      <c r="X27" s="50"/>
+      <c r="Y27" s="51"/>
+      <c r="Z27" s="23"/>
     </row>
     <row r="28" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="40" t="n">
+      <c r="B28" s="42" t="n">
         <v>22</v>
       </c>
-      <c r="C28" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" s="21"/>
+      <c r="C28" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="23"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="40"/>
-      <c r="K28" s="44"/>
-      <c r="L28" s="39"/>
-      <c r="M28" s="45"/>
-      <c r="N28" s="44"/>
-      <c r="O28" s="21"/>
-      <c r="P28" s="45"/>
-      <c r="S28" s="46"/>
-      <c r="T28" s="47"/>
-      <c r="U28" s="48"/>
-      <c r="V28" s="48"/>
-      <c r="W28" s="48"/>
-      <c r="X28" s="48"/>
-      <c r="Y28" s="49"/>
-      <c r="Z28" s="21"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="42"/>
+      <c r="K28" s="46"/>
+      <c r="L28" s="41"/>
+      <c r="M28" s="47"/>
+      <c r="N28" s="46"/>
+      <c r="O28" s="23"/>
+      <c r="P28" s="47"/>
+      <c r="S28" s="48"/>
+      <c r="T28" s="49"/>
+      <c r="U28" s="50"/>
+      <c r="V28" s="50"/>
+      <c r="W28" s="50"/>
+      <c r="X28" s="50"/>
+      <c r="Y28" s="51"/>
+      <c r="Z28" s="23"/>
     </row>
     <row r="29" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="40" t="n">
+      <c r="B29" s="42" t="n">
         <v>23</v>
       </c>
-      <c r="C29" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" s="21"/>
+      <c r="C29" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="23"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="40"/>
-      <c r="K29" s="44"/>
-      <c r="L29" s="21"/>
-      <c r="M29" s="45"/>
-      <c r="N29" s="44"/>
-      <c r="O29" s="21"/>
-      <c r="P29" s="45"/>
-      <c r="S29" s="46"/>
-      <c r="T29" s="47"/>
-      <c r="U29" s="48"/>
-      <c r="V29" s="48"/>
-      <c r="W29" s="48"/>
-      <c r="X29" s="48"/>
-      <c r="Y29" s="49"/>
-      <c r="Z29" s="21"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="42"/>
+      <c r="K29" s="46"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="47"/>
+      <c r="N29" s="46"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="47"/>
+      <c r="S29" s="48"/>
+      <c r="T29" s="49"/>
+      <c r="U29" s="50"/>
+      <c r="V29" s="50"/>
+      <c r="W29" s="50"/>
+      <c r="X29" s="50"/>
+      <c r="Y29" s="51"/>
+      <c r="Z29" s="23"/>
     </row>
     <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="40" t="n">
+      <c r="B30" s="42" t="n">
         <v>24</v>
       </c>
-      <c r="C30" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D30" s="21"/>
+      <c r="C30" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="23"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="43"/>
-      <c r="J30" s="40"/>
-      <c r="K30" s="44"/>
-      <c r="L30" s="21"/>
-      <c r="M30" s="45"/>
-      <c r="N30" s="44"/>
-      <c r="O30" s="21"/>
-      <c r="P30" s="45"/>
-      <c r="S30" s="46"/>
-      <c r="T30" s="47"/>
-      <c r="U30" s="48"/>
-      <c r="V30" s="48"/>
-      <c r="W30" s="48"/>
-      <c r="X30" s="48"/>
-      <c r="Y30" s="49"/>
-      <c r="Z30" s="21"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="42"/>
+      <c r="K30" s="46"/>
+      <c r="L30" s="23"/>
+      <c r="M30" s="47"/>
+      <c r="N30" s="46"/>
+      <c r="O30" s="23"/>
+      <c r="P30" s="47"/>
+      <c r="S30" s="48"/>
+      <c r="T30" s="49"/>
+      <c r="U30" s="50"/>
+      <c r="V30" s="50"/>
+      <c r="W30" s="50"/>
+      <c r="X30" s="50"/>
+      <c r="Y30" s="51"/>
+      <c r="Z30" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:Y1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H2:I2"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="H4:J4"/>
@@ -1990,7 +2037,7 @@
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6:C30" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2 J2 C6:C30" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
telemetry and several small bug fixes and refactorings
</commit_message>
<xml_diff>
--- a/startup/wheel_template.xlsx
+++ b/startup/wheel_template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
   <si>
     <t xml:space="preserve">Experimenters:</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add element to filename?</t>
   </si>
   <si>
     <t xml:space="preserve">File name</t>
@@ -453,7 +456,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -480,6 +483,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -745,9 +752,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1226880</xdr:colOff>
+      <xdr:colOff>1226520</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>60480</xdr:rowOff>
+      <xdr:rowOff>60120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -761,7 +768,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="6933960"/>
-          <a:ext cx="2517480" cy="2743560"/>
+          <a:ext cx="2517480" cy="2743200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -782,9 +789,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>825840</xdr:colOff>
+      <xdr:colOff>825480</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -793,8 +800,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3189600" y="6959880"/>
-          <a:ext cx="6644880" cy="1811160"/>
+          <a:off x="3190320" y="6959880"/>
+          <a:ext cx="6645600" cy="1810800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1010,23 +1017,26 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="M10" activeCellId="0" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="0" width="29.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="14" style="0" width="22.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="17" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="25" min="20" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="25" min="20" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="26" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1073,926 +1083,931 @@
       <c r="J2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="8"/>
+      <c r="K2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="9"/>
       <c r="U2" s="0"/>
       <c r="V2" s="0"/>
       <c r="W2" s="0"/>
       <c r="X2" s="0"/>
-      <c r="Y2" s="8"/>
+      <c r="Y2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="8"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="9"/>
       <c r="U3" s="0"/>
       <c r="V3" s="0"/>
       <c r="W3" s="0"/>
       <c r="X3" s="0"/>
-      <c r="Y3" s="8"/>
+      <c r="Y3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
-      <c r="C4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="10" t="s">
+      <c r="C4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="11" t="s">
+      <c r="D4" s="10"/>
+      <c r="E4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="12" t="s">
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12" t="s">
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12" t="s">
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12" t="s">
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="U4" s="12"/>
-      <c r="V4" s="12"/>
-      <c r="W4" s="12"/>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="12"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="U4" s="13"/>
+      <c r="V4" s="13"/>
+      <c r="W4" s="13"/>
+      <c r="X4" s="13"/>
+      <c r="Y4" s="13"/>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="14" t="s">
+      <c r="B5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="C5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="D5" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="E5" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="F5" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="G5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="H5" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="18" t="s">
+      <c r="I5" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="J5" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="K5" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="20" t="s">
+      <c r="L5" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="N5" s="19" t="s">
+      <c r="M5" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="O5" s="15" t="s">
+      <c r="N5" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="P5" s="20" t="s">
+      <c r="O5" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="Q5" s="21" t="s">
+      <c r="P5" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="R5" s="15" t="s">
+      <c r="Q5" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="S5" s="20" t="s">
+      <c r="R5" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="T5" s="14" t="s">
+      <c r="S5" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="U5" s="13" t="s">
+      <c r="T5" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="V5" s="13" t="s">
+      <c r="U5" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="W5" s="13" t="s">
+      <c r="V5" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="X5" s="13" t="s">
+      <c r="W5" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="Y5" s="18" t="s">
+      <c r="X5" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="Z5" s="22"/>
-    </row>
-    <row r="6" s="23" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="24" t="s">
+      <c r="Y5" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="26" t="s">
+      <c r="Z5" s="23"/>
+    </row>
+    <row r="6" s="24" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="24" t="n">
+      <c r="C6" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="F6" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="27" t="s">
+      <c r="F6" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="28" t="s">
+      <c r="G6" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="29" t="s">
+      <c r="H6" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="30" t="s">
+      <c r="I6" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="K6" s="31" t="s">
+      <c r="J6" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="L6" s="32" t="s">
+      <c r="K6" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="M6" s="33" t="s">
+      <c r="L6" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="N6" s="34" t="s">
+      <c r="M6" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="O6" s="35" t="s">
+      <c r="N6" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="P6" s="36" t="s">
+      <c r="O6" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="Q6" s="37"/>
-      <c r="R6" s="36"/>
-      <c r="S6" s="36"/>
-      <c r="T6" s="38" t="n">
+      <c r="P6" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q6" s="38"/>
+      <c r="R6" s="37"/>
+      <c r="S6" s="37"/>
+      <c r="T6" s="39" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U6" s="39" t="n">
+      <c r="U6" s="40" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="V6" s="39" t="n">
+      <c r="V6" s="40" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="W6" s="39" t="n">
+      <c r="W6" s="40" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="X6" s="39" t="n">
+      <c r="X6" s="40" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Y6" s="40" t="n">
+      <c r="Y6" s="41" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z6" s="41"/>
+      <c r="Z6" s="42"/>
       <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="42" t="n">
+      <c r="B7" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="41"/>
+      <c r="C7" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="42"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="47"/>
-      <c r="N7" s="46"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="47"/>
-      <c r="S7" s="48"/>
-      <c r="T7" s="49"/>
-      <c r="U7" s="50"/>
-      <c r="V7" s="50"/>
-      <c r="W7" s="50"/>
-      <c r="X7" s="50"/>
-      <c r="Y7" s="51"/>
-      <c r="Z7" s="23"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="47"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="48"/>
+      <c r="S7" s="49"/>
+      <c r="T7" s="50"/>
+      <c r="U7" s="51"/>
+      <c r="V7" s="51"/>
+      <c r="W7" s="51"/>
+      <c r="X7" s="51"/>
+      <c r="Y7" s="52"/>
+      <c r="Z7" s="24"/>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="42" t="n">
+      <c r="B8" s="43" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="41"/>
+      <c r="C8" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="42"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="46"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="47"/>
-      <c r="S8" s="48"/>
-      <c r="T8" s="49"/>
-      <c r="U8" s="50"/>
-      <c r="V8" s="50"/>
-      <c r="W8" s="50"/>
-      <c r="X8" s="50"/>
-      <c r="Y8" s="51"/>
-      <c r="Z8" s="23"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="47"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="48"/>
+      <c r="S8" s="49"/>
+      <c r="T8" s="50"/>
+      <c r="U8" s="51"/>
+      <c r="V8" s="51"/>
+      <c r="W8" s="51"/>
+      <c r="X8" s="51"/>
+      <c r="Y8" s="52"/>
+      <c r="Z8" s="24"/>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="42" t="n">
+      <c r="B9" s="43" t="n">
         <v>3</v>
       </c>
-      <c r="C9" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="23"/>
+      <c r="C9" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="24"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="42"/>
-      <c r="K9" s="46"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="47"/>
-      <c r="N9" s="46"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="47"/>
-      <c r="S9" s="48"/>
-      <c r="T9" s="49"/>
-      <c r="U9" s="50"/>
-      <c r="V9" s="50"/>
-      <c r="W9" s="50"/>
-      <c r="X9" s="50"/>
-      <c r="Y9" s="51"/>
-      <c r="Z9" s="23"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="48"/>
+      <c r="N9" s="47"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="48"/>
+      <c r="S9" s="49"/>
+      <c r="T9" s="50"/>
+      <c r="U9" s="51"/>
+      <c r="V9" s="51"/>
+      <c r="W9" s="51"/>
+      <c r="X9" s="51"/>
+      <c r="Y9" s="52"/>
+      <c r="Z9" s="24"/>
     </row>
     <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="42" t="n">
-        <v>4</v>
-      </c>
-      <c r="C10" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="23"/>
+      <c r="B10" s="43" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="24"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="46"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="46"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="47"/>
-      <c r="S10" s="48"/>
-      <c r="T10" s="49"/>
-      <c r="U10" s="50"/>
-      <c r="V10" s="50"/>
-      <c r="W10" s="50"/>
-      <c r="X10" s="50"/>
-      <c r="Y10" s="51"/>
-      <c r="Z10" s="23"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="48"/>
+      <c r="S10" s="49"/>
+      <c r="T10" s="50"/>
+      <c r="U10" s="51"/>
+      <c r="V10" s="51"/>
+      <c r="W10" s="51"/>
+      <c r="X10" s="51"/>
+      <c r="Y10" s="52"/>
+      <c r="Z10" s="24"/>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="42" t="n">
+      <c r="B11" s="43" t="n">
         <v>5</v>
       </c>
-      <c r="C11" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="23"/>
+      <c r="C11" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="24"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="46"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="47"/>
-      <c r="N11" s="46"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="47"/>
-      <c r="S11" s="48"/>
-      <c r="T11" s="49"/>
-      <c r="U11" s="50"/>
-      <c r="V11" s="50"/>
-      <c r="W11" s="50"/>
-      <c r="X11" s="50"/>
-      <c r="Y11" s="51"/>
-      <c r="Z11" s="23"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="48"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="48"/>
+      <c r="S11" s="49"/>
+      <c r="T11" s="50"/>
+      <c r="U11" s="51"/>
+      <c r="V11" s="51"/>
+      <c r="W11" s="51"/>
+      <c r="X11" s="51"/>
+      <c r="Y11" s="52"/>
+      <c r="Z11" s="24"/>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="42" t="n">
+      <c r="B12" s="43" t="n">
         <v>6</v>
       </c>
-      <c r="C12" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="23"/>
+      <c r="C12" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="24"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="46"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="47"/>
-      <c r="N12" s="46"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="47"/>
-      <c r="S12" s="48"/>
-      <c r="T12" s="49"/>
-      <c r="U12" s="50"/>
-      <c r="V12" s="50"/>
-      <c r="W12" s="50"/>
-      <c r="X12" s="50"/>
-      <c r="Y12" s="51"/>
-      <c r="Z12" s="23"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="48"/>
+      <c r="S12" s="49"/>
+      <c r="T12" s="50"/>
+      <c r="U12" s="51"/>
+      <c r="V12" s="51"/>
+      <c r="W12" s="51"/>
+      <c r="X12" s="51"/>
+      <c r="Y12" s="52"/>
+      <c r="Z12" s="24"/>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="42" t="n">
+      <c r="B13" s="43" t="n">
         <v>7</v>
       </c>
-      <c r="C13" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="23"/>
+      <c r="C13" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="24"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="42"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="47"/>
-      <c r="N13" s="46"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="47"/>
-      <c r="S13" s="48"/>
-      <c r="T13" s="49"/>
-      <c r="U13" s="50"/>
-      <c r="V13" s="50"/>
-      <c r="W13" s="50"/>
-      <c r="X13" s="50"/>
-      <c r="Y13" s="51"/>
-      <c r="Z13" s="23"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="47"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="48"/>
+      <c r="S13" s="49"/>
+      <c r="T13" s="50"/>
+      <c r="U13" s="51"/>
+      <c r="V13" s="51"/>
+      <c r="W13" s="51"/>
+      <c r="X13" s="51"/>
+      <c r="Y13" s="52"/>
+      <c r="Z13" s="24"/>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="42" t="n">
+      <c r="B14" s="43" t="n">
         <v>8</v>
       </c>
-      <c r="C14" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="23"/>
+      <c r="C14" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="24"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="45"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="46"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="47"/>
-      <c r="N14" s="46"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="47"/>
-      <c r="S14" s="48"/>
-      <c r="T14" s="49"/>
-      <c r="U14" s="50"/>
-      <c r="V14" s="50"/>
-      <c r="W14" s="50"/>
-      <c r="X14" s="50"/>
-      <c r="Y14" s="51"/>
-      <c r="Z14" s="23"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="47"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="48"/>
+      <c r="S14" s="49"/>
+      <c r="T14" s="50"/>
+      <c r="U14" s="51"/>
+      <c r="V14" s="51"/>
+      <c r="W14" s="51"/>
+      <c r="X14" s="51"/>
+      <c r="Y14" s="52"/>
+      <c r="Z14" s="24"/>
     </row>
     <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="42" t="n">
+      <c r="B15" s="43" t="n">
         <v>9</v>
       </c>
-      <c r="C15" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="23"/>
+      <c r="C15" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="24"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="45"/>
-      <c r="J15" s="42"/>
-      <c r="K15" s="46"/>
-      <c r="L15" s="41"/>
-      <c r="M15" s="47"/>
-      <c r="N15" s="46"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="47"/>
-      <c r="S15" s="48"/>
-      <c r="T15" s="49"/>
-      <c r="U15" s="50"/>
-      <c r="V15" s="50"/>
-      <c r="W15" s="50"/>
-      <c r="X15" s="50"/>
-      <c r="Y15" s="51"/>
-      <c r="Z15" s="23"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="48"/>
+      <c r="N15" s="47"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="48"/>
+      <c r="S15" s="49"/>
+      <c r="T15" s="50"/>
+      <c r="U15" s="51"/>
+      <c r="V15" s="51"/>
+      <c r="W15" s="51"/>
+      <c r="X15" s="51"/>
+      <c r="Y15" s="52"/>
+      <c r="Z15" s="24"/>
     </row>
     <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="42" t="n">
+      <c r="B16" s="43" t="n">
         <v>10</v>
       </c>
-      <c r="C16" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="23"/>
+      <c r="C16" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="24"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="45"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="46"/>
-      <c r="L16" s="41"/>
-      <c r="M16" s="47"/>
-      <c r="N16" s="46"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="47"/>
-      <c r="S16" s="48"/>
-      <c r="T16" s="49"/>
-      <c r="U16" s="50"/>
-      <c r="V16" s="50"/>
-      <c r="W16" s="50"/>
-      <c r="X16" s="50"/>
-      <c r="Y16" s="51"/>
-      <c r="Z16" s="23"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="48"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="48"/>
+      <c r="S16" s="49"/>
+      <c r="T16" s="50"/>
+      <c r="U16" s="51"/>
+      <c r="V16" s="51"/>
+      <c r="W16" s="51"/>
+      <c r="X16" s="51"/>
+      <c r="Y16" s="52"/>
+      <c r="Z16" s="24"/>
     </row>
     <row r="17" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="42" t="n">
+      <c r="B17" s="43" t="n">
         <v>11</v>
       </c>
-      <c r="C17" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="23"/>
+      <c r="C17" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="24"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="42"/>
-      <c r="K17" s="46"/>
-      <c r="L17" s="41"/>
-      <c r="M17" s="47"/>
-      <c r="N17" s="46"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="47"/>
-      <c r="S17" s="48"/>
-      <c r="T17" s="49"/>
-      <c r="U17" s="50"/>
-      <c r="V17" s="50"/>
-      <c r="W17" s="50"/>
-      <c r="X17" s="50"/>
-      <c r="Y17" s="51"/>
-      <c r="Z17" s="23"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="42"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="47"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="48"/>
+      <c r="S17" s="49"/>
+      <c r="T17" s="50"/>
+      <c r="U17" s="51"/>
+      <c r="V17" s="51"/>
+      <c r="W17" s="51"/>
+      <c r="X17" s="51"/>
+      <c r="Y17" s="52"/>
+      <c r="Z17" s="24"/>
     </row>
     <row r="18" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="42" t="n">
+      <c r="B18" s="43" t="n">
         <v>12</v>
       </c>
-      <c r="C18" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="23"/>
+      <c r="C18" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="24"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="45"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="46"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="47"/>
-      <c r="N18" s="46"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="47"/>
-      <c r="S18" s="48"/>
-      <c r="T18" s="49"/>
-      <c r="U18" s="50"/>
-      <c r="V18" s="50"/>
-      <c r="W18" s="50"/>
-      <c r="X18" s="50"/>
-      <c r="Y18" s="51"/>
-      <c r="Z18" s="23"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="47"/>
+      <c r="L18" s="42"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="47"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="48"/>
+      <c r="S18" s="49"/>
+      <c r="T18" s="50"/>
+      <c r="U18" s="51"/>
+      <c r="V18" s="51"/>
+      <c r="W18" s="51"/>
+      <c r="X18" s="51"/>
+      <c r="Y18" s="52"/>
+      <c r="Z18" s="24"/>
     </row>
     <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="42" t="n">
+      <c r="B19" s="43" t="n">
         <v>13</v>
       </c>
-      <c r="C19" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="23"/>
+      <c r="C19" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="24"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="42"/>
-      <c r="K19" s="46"/>
-      <c r="L19" s="41"/>
-      <c r="M19" s="47"/>
-      <c r="N19" s="46"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="47"/>
-      <c r="S19" s="48"/>
-      <c r="T19" s="49"/>
-      <c r="U19" s="50"/>
-      <c r="V19" s="50"/>
-      <c r="W19" s="50"/>
-      <c r="X19" s="50"/>
-      <c r="Y19" s="51"/>
-      <c r="Z19" s="23"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="47"/>
+      <c r="L19" s="42"/>
+      <c r="M19" s="48"/>
+      <c r="N19" s="47"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="48"/>
+      <c r="S19" s="49"/>
+      <c r="T19" s="50"/>
+      <c r="U19" s="51"/>
+      <c r="V19" s="51"/>
+      <c r="W19" s="51"/>
+      <c r="X19" s="51"/>
+      <c r="Y19" s="52"/>
+      <c r="Z19" s="24"/>
     </row>
     <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="42" t="n">
+      <c r="B20" s="43" t="n">
         <v>14</v>
       </c>
-      <c r="C20" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="23"/>
+      <c r="C20" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="24"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="46"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="47"/>
-      <c r="N20" s="46"/>
-      <c r="O20" s="23"/>
-      <c r="P20" s="47"/>
-      <c r="S20" s="48"/>
-      <c r="T20" s="49"/>
-      <c r="U20" s="50"/>
-      <c r="V20" s="50"/>
-      <c r="W20" s="50"/>
-      <c r="X20" s="50"/>
-      <c r="Y20" s="51"/>
-      <c r="Z20" s="23"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="47"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="48"/>
+      <c r="S20" s="49"/>
+      <c r="T20" s="50"/>
+      <c r="U20" s="51"/>
+      <c r="V20" s="51"/>
+      <c r="W20" s="51"/>
+      <c r="X20" s="51"/>
+      <c r="Y20" s="52"/>
+      <c r="Z20" s="24"/>
     </row>
     <row r="21" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="42" t="n">
+      <c r="B21" s="43" t="n">
         <v>15</v>
       </c>
-      <c r="C21" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="23"/>
+      <c r="C21" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="24"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="45"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="46"/>
-      <c r="L21" s="41"/>
-      <c r="M21" s="47"/>
-      <c r="N21" s="46"/>
-      <c r="O21" s="23"/>
-      <c r="P21" s="47"/>
-      <c r="S21" s="48"/>
-      <c r="T21" s="49"/>
-      <c r="U21" s="50"/>
-      <c r="V21" s="50"/>
-      <c r="W21" s="50"/>
-      <c r="X21" s="50"/>
-      <c r="Y21" s="51"/>
-      <c r="Z21" s="23"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="42"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="47"/>
+      <c r="O21" s="24"/>
+      <c r="P21" s="48"/>
+      <c r="S21" s="49"/>
+      <c r="T21" s="50"/>
+      <c r="U21" s="51"/>
+      <c r="V21" s="51"/>
+      <c r="W21" s="51"/>
+      <c r="X21" s="51"/>
+      <c r="Y21" s="52"/>
+      <c r="Z21" s="24"/>
     </row>
     <row r="22" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="42" t="n">
+      <c r="B22" s="43" t="n">
         <v>16</v>
       </c>
-      <c r="C22" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="23"/>
+      <c r="C22" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="24"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="45"/>
-      <c r="J22" s="42"/>
-      <c r="K22" s="46"/>
-      <c r="L22" s="41"/>
-      <c r="M22" s="47"/>
-      <c r="N22" s="46"/>
-      <c r="O22" s="23"/>
-      <c r="P22" s="47"/>
-      <c r="S22" s="48"/>
-      <c r="T22" s="49"/>
-      <c r="U22" s="50"/>
-      <c r="V22" s="50"/>
-      <c r="W22" s="50"/>
-      <c r="X22" s="50"/>
-      <c r="Y22" s="51"/>
-      <c r="Z22" s="23"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="47"/>
+      <c r="L22" s="42"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="47"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="48"/>
+      <c r="S22" s="49"/>
+      <c r="T22" s="50"/>
+      <c r="U22" s="51"/>
+      <c r="V22" s="51"/>
+      <c r="W22" s="51"/>
+      <c r="X22" s="51"/>
+      <c r="Y22" s="52"/>
+      <c r="Z22" s="24"/>
     </row>
     <row r="23" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="42" t="n">
+      <c r="B23" s="43" t="n">
         <v>17</v>
       </c>
-      <c r="C23" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="23"/>
+      <c r="C23" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="24"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="42"/>
-      <c r="K23" s="46"/>
-      <c r="L23" s="41"/>
-      <c r="M23" s="47"/>
-      <c r="N23" s="46"/>
-      <c r="O23" s="23"/>
-      <c r="P23" s="47"/>
-      <c r="S23" s="48"/>
-      <c r="T23" s="49"/>
-      <c r="U23" s="50"/>
-      <c r="V23" s="50"/>
-      <c r="W23" s="50"/>
-      <c r="X23" s="50"/>
-      <c r="Y23" s="51"/>
-      <c r="Z23" s="23"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="43"/>
+      <c r="K23" s="47"/>
+      <c r="L23" s="42"/>
+      <c r="M23" s="48"/>
+      <c r="N23" s="47"/>
+      <c r="O23" s="24"/>
+      <c r="P23" s="48"/>
+      <c r="S23" s="49"/>
+      <c r="T23" s="50"/>
+      <c r="U23" s="51"/>
+      <c r="V23" s="51"/>
+      <c r="W23" s="51"/>
+      <c r="X23" s="51"/>
+      <c r="Y23" s="52"/>
+      <c r="Z23" s="24"/>
     </row>
     <row r="24" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="42" t="n">
+      <c r="B24" s="43" t="n">
         <v>18</v>
       </c>
-      <c r="C24" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="23"/>
+      <c r="C24" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="24"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="46"/>
-      <c r="L24" s="41"/>
-      <c r="M24" s="47"/>
-      <c r="N24" s="46"/>
-      <c r="O24" s="23"/>
-      <c r="P24" s="47"/>
-      <c r="S24" s="48"/>
-      <c r="T24" s="49"/>
-      <c r="U24" s="50"/>
-      <c r="V24" s="50"/>
-      <c r="W24" s="50"/>
-      <c r="X24" s="50"/>
-      <c r="Y24" s="51"/>
-      <c r="Z24" s="23"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="43"/>
+      <c r="K24" s="47"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="48"/>
+      <c r="N24" s="47"/>
+      <c r="O24" s="24"/>
+      <c r="P24" s="48"/>
+      <c r="S24" s="49"/>
+      <c r="T24" s="50"/>
+      <c r="U24" s="51"/>
+      <c r="V24" s="51"/>
+      <c r="W24" s="51"/>
+      <c r="X24" s="51"/>
+      <c r="Y24" s="52"/>
+      <c r="Z24" s="24"/>
     </row>
     <row r="25" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="42" t="n">
+      <c r="B25" s="43" t="n">
         <v>19</v>
       </c>
-      <c r="C25" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="23"/>
+      <c r="C25" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="24"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="45"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="46"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="47"/>
-      <c r="N25" s="46"/>
-      <c r="O25" s="23"/>
-      <c r="P25" s="47"/>
-      <c r="S25" s="48"/>
-      <c r="T25" s="49"/>
-      <c r="U25" s="50"/>
-      <c r="V25" s="50"/>
-      <c r="W25" s="50"/>
-      <c r="X25" s="50"/>
-      <c r="Y25" s="51"/>
-      <c r="Z25" s="23"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="47"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="48"/>
+      <c r="N25" s="47"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="48"/>
+      <c r="S25" s="49"/>
+      <c r="T25" s="50"/>
+      <c r="U25" s="51"/>
+      <c r="V25" s="51"/>
+      <c r="W25" s="51"/>
+      <c r="X25" s="51"/>
+      <c r="Y25" s="52"/>
+      <c r="Z25" s="24"/>
     </row>
     <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="42" t="n">
+      <c r="B26" s="43" t="n">
         <v>20</v>
       </c>
-      <c r="C26" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="23"/>
+      <c r="C26" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="24"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
-      <c r="H26" s="44"/>
-      <c r="I26" s="45"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="46"/>
-      <c r="L26" s="41"/>
-      <c r="M26" s="47"/>
-      <c r="N26" s="46"/>
-      <c r="O26" s="23"/>
-      <c r="P26" s="47"/>
-      <c r="S26" s="48"/>
-      <c r="T26" s="49"/>
-      <c r="U26" s="50"/>
-      <c r="V26" s="50"/>
-      <c r="W26" s="50"/>
-      <c r="X26" s="50"/>
-      <c r="Y26" s="51"/>
-      <c r="Z26" s="23"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="47"/>
+      <c r="L26" s="42"/>
+      <c r="M26" s="48"/>
+      <c r="N26" s="47"/>
+      <c r="O26" s="24"/>
+      <c r="P26" s="48"/>
+      <c r="S26" s="49"/>
+      <c r="T26" s="50"/>
+      <c r="U26" s="51"/>
+      <c r="V26" s="51"/>
+      <c r="W26" s="51"/>
+      <c r="X26" s="51"/>
+      <c r="Y26" s="52"/>
+      <c r="Z26" s="24"/>
     </row>
     <row r="27" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="42" t="n">
+      <c r="B27" s="43" t="n">
         <v>21</v>
       </c>
-      <c r="C27" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="23"/>
+      <c r="C27" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="24"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="45"/>
-      <c r="J27" s="42"/>
-      <c r="K27" s="46"/>
-      <c r="L27" s="41"/>
-      <c r="M27" s="47"/>
-      <c r="N27" s="46"/>
-      <c r="O27" s="23"/>
-      <c r="P27" s="47"/>
-      <c r="S27" s="48"/>
-      <c r="T27" s="49"/>
-      <c r="U27" s="50"/>
-      <c r="V27" s="50"/>
-      <c r="W27" s="50"/>
-      <c r="X27" s="50"/>
-      <c r="Y27" s="51"/>
-      <c r="Z27" s="23"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="47"/>
+      <c r="L27" s="42"/>
+      <c r="M27" s="48"/>
+      <c r="N27" s="47"/>
+      <c r="O27" s="24"/>
+      <c r="P27" s="48"/>
+      <c r="S27" s="49"/>
+      <c r="T27" s="50"/>
+      <c r="U27" s="51"/>
+      <c r="V27" s="51"/>
+      <c r="W27" s="51"/>
+      <c r="X27" s="51"/>
+      <c r="Y27" s="52"/>
+      <c r="Z27" s="24"/>
     </row>
     <row r="28" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="42" t="n">
+      <c r="B28" s="43" t="n">
         <v>22</v>
       </c>
-      <c r="C28" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" s="23"/>
+      <c r="C28" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="24"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="42"/>
-      <c r="K28" s="46"/>
-      <c r="L28" s="41"/>
-      <c r="M28" s="47"/>
-      <c r="N28" s="46"/>
-      <c r="O28" s="23"/>
-      <c r="P28" s="47"/>
-      <c r="S28" s="48"/>
-      <c r="T28" s="49"/>
-      <c r="U28" s="50"/>
-      <c r="V28" s="50"/>
-      <c r="W28" s="50"/>
-      <c r="X28" s="50"/>
-      <c r="Y28" s="51"/>
-      <c r="Z28" s="23"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="46"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="47"/>
+      <c r="L28" s="42"/>
+      <c r="M28" s="48"/>
+      <c r="N28" s="47"/>
+      <c r="O28" s="24"/>
+      <c r="P28" s="48"/>
+      <c r="S28" s="49"/>
+      <c r="T28" s="50"/>
+      <c r="U28" s="51"/>
+      <c r="V28" s="51"/>
+      <c r="W28" s="51"/>
+      <c r="X28" s="51"/>
+      <c r="Y28" s="52"/>
+      <c r="Z28" s="24"/>
     </row>
     <row r="29" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="42" t="n">
+      <c r="B29" s="43" t="n">
         <v>23</v>
       </c>
-      <c r="C29" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" s="23"/>
+      <c r="C29" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="24"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="42"/>
-      <c r="K29" s="46"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="47"/>
-      <c r="N29" s="46"/>
-      <c r="O29" s="23"/>
-      <c r="P29" s="47"/>
-      <c r="S29" s="48"/>
-      <c r="T29" s="49"/>
-      <c r="U29" s="50"/>
-      <c r="V29" s="50"/>
-      <c r="W29" s="50"/>
-      <c r="X29" s="50"/>
-      <c r="Y29" s="51"/>
-      <c r="Z29" s="23"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="47"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="48"/>
+      <c r="N29" s="47"/>
+      <c r="O29" s="24"/>
+      <c r="P29" s="48"/>
+      <c r="S29" s="49"/>
+      <c r="T29" s="50"/>
+      <c r="U29" s="51"/>
+      <c r="V29" s="51"/>
+      <c r="W29" s="51"/>
+      <c r="X29" s="51"/>
+      <c r="Y29" s="52"/>
+      <c r="Z29" s="24"/>
     </row>
     <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="42" t="n">
+      <c r="B30" s="43" t="n">
         <v>24</v>
       </c>
-      <c r="C30" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="23"/>
+      <c r="C30" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="24"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="42"/>
-      <c r="K30" s="46"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="47"/>
-      <c r="N30" s="46"/>
-      <c r="O30" s="23"/>
-      <c r="P30" s="47"/>
-      <c r="S30" s="48"/>
-      <c r="T30" s="49"/>
-      <c r="U30" s="50"/>
-      <c r="V30" s="50"/>
-      <c r="W30" s="50"/>
-      <c r="X30" s="50"/>
-      <c r="Y30" s="51"/>
-      <c r="Z30" s="23"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="43"/>
+      <c r="K30" s="47"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="48"/>
+      <c r="N30" s="47"/>
+      <c r="O30" s="24"/>
+      <c r="P30" s="48"/>
+      <c r="S30" s="49"/>
+      <c r="T30" s="50"/>
+      <c r="U30" s="51"/>
+      <c r="V30" s="51"/>
+      <c r="W30" s="51"/>
+      <c r="X30" s="51"/>
+      <c r="Y30" s="52"/>
+      <c r="Z30" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -2008,7 +2023,7 @@
     <mergeCell ref="Q4:S4"/>
     <mergeCell ref="T4:Y4"/>
   </mergeCells>
-  <dataValidations count="13">
+  <dataValidations count="14">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T6:Y30" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
@@ -2061,6 +2076,10 @@
       <formula1>-150</formula1>
       <formula2>150</formula2>
     </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
+      <formula1>"No,Beginning,End"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
work in support of remote ops
* migrate use of abs_set() to mv()
* kw of 2 bkg removal in larch,py
* use start.XDI._dtc to figure out how make fluo xas
* add BMMuser.lims attribute for shutting off entire lims system
* write XRF files and images to XRF folder
* compute total time on wheel correctly
* add OCR and ROI count rates at Eave to dossier
* add XDI metadata to start doc of XRF and snapshots
* prototype for autobackup to Google drive
* make BMM/db.py for DataBroker related stuff, tool for fetching a file resource
* move from rois.ini to rois.json
* better title in XRF plot
</commit_message>
<xml_diff>
--- a/startup/wheel_template.xlsx
+++ b/startup/wheel_template.xlsx
@@ -752,9 +752,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1226520</xdr:colOff>
+      <xdr:colOff>1226160</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>60120</xdr:rowOff>
+      <xdr:rowOff>59760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -768,7 +768,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="6933960"/>
-          <a:ext cx="2517480" cy="2743200"/>
+          <a:ext cx="2516760" cy="2742840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -789,9 +789,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>825480</xdr:colOff>
+      <xdr:colOff>825120</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>129240</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -800,8 +800,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3190320" y="6959880"/>
-          <a:ext cx="6645600" cy="1810800"/>
+          <a:off x="3189600" y="6959880"/>
+          <a:ext cx="6644880" cy="1810440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1017,7 +1017,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="M10" activeCellId="0" sqref="M10"/>
+      <selection pane="bottomRight" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2023,7 +2023,7 @@
     <mergeCell ref="Q4:S4"/>
     <mergeCell ref="T4:Y4"/>
   </mergeCells>
-  <dataValidations count="14">
+  <dataValidations count="15">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T6:Y30" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
@@ -2034,10 +2034,6 @@
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J30" type="list">
       <formula1>"unfocused,focused"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6:G30" type="list">
-      <formula1>"transmission,fluorescence,both,reference,yield,test"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6:H30" type="list">
@@ -2080,6 +2076,14 @@
       <formula1>"No,Beginning,End"</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6" type="list">
+      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G7:G30" type="list">
+      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
more work related to remote
* implement controls for 1-element vortex
* separate objects for 4- and 1-element
* reference in larch.py
* tweak gdrive functionality
* add url, cif, doi to spreadsheet, ini file, & dossier
</commit_message>
<xml_diff>
--- a/startup/wheel_template.xlsx
+++ b/startup/wheel_template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
   <si>
     <t xml:space="preserve">Experimenters:</t>
   </si>
@@ -61,6 +61,9 @@
     <t xml:space="preserve">Flags</t>
   </si>
   <si>
+    <t xml:space="preserve">Ancillary information</t>
+  </si>
+  <si>
     <t xml:space="preserve">Slot number</t>
   </si>
   <si>
@@ -131,6 +134,15 @@
   </si>
   <si>
     <t xml:space="preserve">ththth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIF</t>
   </si>
   <si>
     <t xml:space="preserve">Default</t>
@@ -257,7 +269,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -430,6 +442,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -456,7 +479,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -513,6 +536,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -549,8 +576,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -625,18 +652,22 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -667,6 +698,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -752,9 +787,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1226160</xdr:colOff>
+      <xdr:colOff>1225800</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>59760</xdr:rowOff>
+      <xdr:rowOff>59400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -768,7 +803,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="6933960"/>
-          <a:ext cx="2516760" cy="2742840"/>
+          <a:ext cx="2516400" cy="2742480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -789,9 +824,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>825120</xdr:colOff>
+      <xdr:colOff>824760</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>128880</xdr:rowOff>
+      <xdr:rowOff>128520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -801,7 +836,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3189600" y="6959880"/>
-          <a:ext cx="6644880" cy="1810440"/>
+          <a:ext cx="6644520" cy="1810080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1013,11 +1048,11 @@
   <dimension ref="B1:AMJ30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="6" topLeftCell="O7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topRight" activeCell="O1" activeCellId="0" sqref="O1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="F16" activeCellId="0" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="Z9" activeCellId="0" sqref="Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1036,7 +1071,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="14" style="0" width="22.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="17" style="0" width="14.43"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="25" min="20" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="26" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="27.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="29" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1161,856 +1199,871 @@
       <c r="W4" s="13"/>
       <c r="X4" s="13"/>
       <c r="Y4" s="13"/>
+      <c r="Z4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA4" s="14"/>
+      <c r="AB4" s="14"/>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="15" t="s">
+      <c r="B5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="C5" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="D5" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="E5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="F5" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="G5" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="H5" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="I5" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="20" t="s">
+      <c r="J5" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="16" t="s">
+      <c r="K5" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="M5" s="21" t="s">
+      <c r="L5" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="N5" s="20" t="s">
+      <c r="M5" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="O5" s="16" t="s">
+      <c r="N5" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="P5" s="21" t="s">
+      <c r="O5" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="Q5" s="22" t="s">
+      <c r="P5" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="R5" s="16" t="s">
+      <c r="Q5" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="S5" s="21" t="s">
+      <c r="R5" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="T5" s="15" t="s">
+      <c r="S5" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="U5" s="14" t="s">
+      <c r="T5" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="V5" s="14" t="s">
+      <c r="U5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="W5" s="14" t="s">
+      <c r="V5" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="X5" s="14" t="s">
+      <c r="W5" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="Y5" s="19" t="s">
+      <c r="X5" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="Z5" s="23"/>
-    </row>
-    <row r="6" s="24" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="25" t="s">
+      <c r="Y5" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="27" t="s">
+      <c r="Z5" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="25" t="n">
+      <c r="AA5" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB5" s="24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" s="25" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B6" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="F6" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="I6" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="J6" s="31" t="s">
+      <c r="F6" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="K6" s="32" t="s">
+      <c r="G6" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="L6" s="33" t="s">
+      <c r="H6" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="M6" s="34" t="s">
+      <c r="I6" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="N6" s="35" t="s">
+      <c r="J6" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="O6" s="36" t="s">
+      <c r="K6" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="P6" s="37" t="s">
+      <c r="L6" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="Q6" s="38"/>
-      <c r="R6" s="37"/>
-      <c r="S6" s="37"/>
-      <c r="T6" s="39" t="n">
+      <c r="M6" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="N6" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="O6" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="P6" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q6" s="39"/>
+      <c r="R6" s="38"/>
+      <c r="S6" s="38"/>
+      <c r="T6" s="40" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U6" s="40" t="n">
+      <c r="U6" s="41" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="V6" s="40" t="n">
+      <c r="V6" s="41" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="W6" s="40" t="n">
+      <c r="W6" s="41" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="X6" s="40" t="n">
+      <c r="X6" s="41" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Y6" s="41" t="n">
+      <c r="Y6" s="42" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z6" s="42"/>
+      <c r="Z6" s="43"/>
+      <c r="AA6" s="38"/>
+      <c r="AB6" s="38"/>
       <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="43" t="n">
+      <c r="B7" s="44" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="42"/>
+      <c r="C7" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="46"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="47"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="48"/>
-      <c r="N7" s="47"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="48"/>
-      <c r="S7" s="49"/>
-      <c r="T7" s="50"/>
-      <c r="U7" s="51"/>
-      <c r="V7" s="51"/>
-      <c r="W7" s="51"/>
-      <c r="X7" s="51"/>
-      <c r="Y7" s="52"/>
-      <c r="Z7" s="24"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="50"/>
+      <c r="S7" s="51"/>
+      <c r="T7" s="52"/>
+      <c r="U7" s="53"/>
+      <c r="V7" s="53"/>
+      <c r="W7" s="53"/>
+      <c r="X7" s="53"/>
+      <c r="Y7" s="54"/>
+      <c r="Z7" s="55"/>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="43" t="n">
+      <c r="B8" s="44" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="42"/>
+      <c r="C8" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="46"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="48"/>
-      <c r="N8" s="47"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="48"/>
-      <c r="S8" s="49"/>
-      <c r="T8" s="50"/>
-      <c r="U8" s="51"/>
-      <c r="V8" s="51"/>
-      <c r="W8" s="51"/>
-      <c r="X8" s="51"/>
-      <c r="Y8" s="52"/>
-      <c r="Z8" s="24"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="49"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="50"/>
+      <c r="S8" s="51"/>
+      <c r="T8" s="52"/>
+      <c r="U8" s="53"/>
+      <c r="V8" s="53"/>
+      <c r="W8" s="53"/>
+      <c r="X8" s="53"/>
+      <c r="Y8" s="54"/>
+      <c r="Z8" s="55"/>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="43" t="n">
+      <c r="B9" s="44" t="n">
         <v>3</v>
       </c>
-      <c r="C9" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="24"/>
+      <c r="C9" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="25"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="46"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="42"/>
-      <c r="M9" s="48"/>
-      <c r="N9" s="47"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="48"/>
-      <c r="S9" s="49"/>
-      <c r="T9" s="50"/>
-      <c r="U9" s="51"/>
-      <c r="V9" s="51"/>
-      <c r="W9" s="51"/>
-      <c r="X9" s="51"/>
-      <c r="Y9" s="52"/>
-      <c r="Z9" s="24"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="50"/>
+      <c r="N9" s="49"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="50"/>
+      <c r="S9" s="51"/>
+      <c r="T9" s="52"/>
+      <c r="U9" s="53"/>
+      <c r="V9" s="53"/>
+      <c r="W9" s="53"/>
+      <c r="X9" s="53"/>
+      <c r="Y9" s="54"/>
+      <c r="Z9" s="55"/>
     </row>
     <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="43" t="n">
-        <v>4</v>
-      </c>
-      <c r="C10" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="24"/>
+      <c r="B10" s="44" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="25"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="47"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="48"/>
-      <c r="N10" s="47"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="48"/>
-      <c r="S10" s="49"/>
-      <c r="T10" s="50"/>
-      <c r="U10" s="51"/>
-      <c r="V10" s="51"/>
-      <c r="W10" s="51"/>
-      <c r="X10" s="51"/>
-      <c r="Y10" s="52"/>
-      <c r="Z10" s="24"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="49"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="50"/>
+      <c r="S10" s="51"/>
+      <c r="T10" s="52"/>
+      <c r="U10" s="53"/>
+      <c r="V10" s="53"/>
+      <c r="W10" s="53"/>
+      <c r="X10" s="53"/>
+      <c r="Y10" s="54"/>
+      <c r="Z10" s="55"/>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="43" t="n">
+      <c r="B11" s="44" t="n">
         <v>5</v>
       </c>
-      <c r="C11" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="24"/>
+      <c r="C11" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="25"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="47"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="48"/>
-      <c r="N11" s="47"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="48"/>
-      <c r="S11" s="49"/>
-      <c r="T11" s="50"/>
-      <c r="U11" s="51"/>
-      <c r="V11" s="51"/>
-      <c r="W11" s="51"/>
-      <c r="X11" s="51"/>
-      <c r="Y11" s="52"/>
-      <c r="Z11" s="24"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="50"/>
+      <c r="N11" s="49"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="50"/>
+      <c r="S11" s="51"/>
+      <c r="T11" s="52"/>
+      <c r="U11" s="53"/>
+      <c r="V11" s="53"/>
+      <c r="W11" s="53"/>
+      <c r="X11" s="53"/>
+      <c r="Y11" s="54"/>
+      <c r="Z11" s="55"/>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="43" t="n">
+      <c r="B12" s="44" t="n">
         <v>6</v>
       </c>
-      <c r="C12" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="24"/>
+      <c r="C12" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="25"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="47"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="48"/>
-      <c r="N12" s="47"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="48"/>
-      <c r="S12" s="49"/>
-      <c r="T12" s="50"/>
-      <c r="U12" s="51"/>
-      <c r="V12" s="51"/>
-      <c r="W12" s="51"/>
-      <c r="X12" s="51"/>
-      <c r="Y12" s="52"/>
-      <c r="Z12" s="24"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="44"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="46"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="49"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="50"/>
+      <c r="S12" s="51"/>
+      <c r="T12" s="52"/>
+      <c r="U12" s="53"/>
+      <c r="V12" s="53"/>
+      <c r="W12" s="53"/>
+      <c r="X12" s="53"/>
+      <c r="Y12" s="54"/>
+      <c r="Z12" s="55"/>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="43" t="n">
+      <c r="B13" s="44" t="n">
         <v>7</v>
       </c>
-      <c r="C13" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="24"/>
+      <c r="C13" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="25"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="47"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="48"/>
-      <c r="N13" s="47"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="48"/>
-      <c r="S13" s="49"/>
-      <c r="T13" s="50"/>
-      <c r="U13" s="51"/>
-      <c r="V13" s="51"/>
-      <c r="W13" s="51"/>
-      <c r="X13" s="51"/>
-      <c r="Y13" s="52"/>
-      <c r="Z13" s="24"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="46"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="49"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="50"/>
+      <c r="S13" s="51"/>
+      <c r="T13" s="52"/>
+      <c r="U13" s="53"/>
+      <c r="V13" s="53"/>
+      <c r="W13" s="53"/>
+      <c r="X13" s="53"/>
+      <c r="Y13" s="54"/>
+      <c r="Z13" s="55"/>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="43" t="n">
+      <c r="B14" s="44" t="n">
         <v>8</v>
       </c>
-      <c r="C14" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="24"/>
+      <c r="C14" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="25"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="47"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="47"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="48"/>
-      <c r="S14" s="49"/>
-      <c r="T14" s="50"/>
-      <c r="U14" s="51"/>
-      <c r="V14" s="51"/>
-      <c r="W14" s="51"/>
-      <c r="X14" s="51"/>
-      <c r="Y14" s="52"/>
-      <c r="Z14" s="24"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="46"/>
+      <c r="M14" s="50"/>
+      <c r="N14" s="49"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="50"/>
+      <c r="S14" s="51"/>
+      <c r="T14" s="52"/>
+      <c r="U14" s="53"/>
+      <c r="V14" s="53"/>
+      <c r="W14" s="53"/>
+      <c r="X14" s="53"/>
+      <c r="Y14" s="54"/>
+      <c r="Z14" s="55"/>
     </row>
     <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="43" t="n">
+      <c r="B15" s="44" t="n">
         <v>9</v>
       </c>
-      <c r="C15" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="24"/>
+      <c r="C15" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="25"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="46"/>
-      <c r="J15" s="43"/>
-      <c r="K15" s="47"/>
-      <c r="L15" s="42"/>
-      <c r="M15" s="48"/>
-      <c r="N15" s="47"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="48"/>
-      <c r="S15" s="49"/>
-      <c r="T15" s="50"/>
-      <c r="U15" s="51"/>
-      <c r="V15" s="51"/>
-      <c r="W15" s="51"/>
-      <c r="X15" s="51"/>
-      <c r="Y15" s="52"/>
-      <c r="Z15" s="24"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="49"/>
+      <c r="L15" s="46"/>
+      <c r="M15" s="50"/>
+      <c r="N15" s="49"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="50"/>
+      <c r="S15" s="51"/>
+      <c r="T15" s="52"/>
+      <c r="U15" s="53"/>
+      <c r="V15" s="53"/>
+      <c r="W15" s="53"/>
+      <c r="X15" s="53"/>
+      <c r="Y15" s="54"/>
+      <c r="Z15" s="55"/>
     </row>
     <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="43" t="n">
+      <c r="B16" s="44" t="n">
         <v>10</v>
       </c>
-      <c r="C16" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="24"/>
+      <c r="C16" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="25"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="46"/>
-      <c r="J16" s="43"/>
-      <c r="K16" s="47"/>
-      <c r="L16" s="42"/>
-      <c r="M16" s="48"/>
-      <c r="N16" s="47"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="48"/>
-      <c r="S16" s="49"/>
-      <c r="T16" s="50"/>
-      <c r="U16" s="51"/>
-      <c r="V16" s="51"/>
-      <c r="W16" s="51"/>
-      <c r="X16" s="51"/>
-      <c r="Y16" s="52"/>
-      <c r="Z16" s="24"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="44"/>
+      <c r="K16" s="49"/>
+      <c r="L16" s="46"/>
+      <c r="M16" s="50"/>
+      <c r="N16" s="49"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="50"/>
+      <c r="S16" s="51"/>
+      <c r="T16" s="52"/>
+      <c r="U16" s="53"/>
+      <c r="V16" s="53"/>
+      <c r="W16" s="53"/>
+      <c r="X16" s="53"/>
+      <c r="Y16" s="54"/>
+      <c r="Z16" s="55"/>
     </row>
     <row r="17" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="43" t="n">
+      <c r="B17" s="44" t="n">
         <v>11</v>
       </c>
-      <c r="C17" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="24"/>
+      <c r="C17" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="25"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="43"/>
-      <c r="K17" s="47"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="47"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="48"/>
-      <c r="S17" s="49"/>
-      <c r="T17" s="50"/>
-      <c r="U17" s="51"/>
-      <c r="V17" s="51"/>
-      <c r="W17" s="51"/>
-      <c r="X17" s="51"/>
-      <c r="Y17" s="52"/>
-      <c r="Z17" s="24"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="49"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="50"/>
+      <c r="N17" s="49"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="50"/>
+      <c r="S17" s="51"/>
+      <c r="T17" s="52"/>
+      <c r="U17" s="53"/>
+      <c r="V17" s="53"/>
+      <c r="W17" s="53"/>
+      <c r="X17" s="53"/>
+      <c r="Y17" s="54"/>
+      <c r="Z17" s="55"/>
     </row>
     <row r="18" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="43" t="n">
+      <c r="B18" s="44" t="n">
         <v>12</v>
       </c>
-      <c r="C18" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="24"/>
+      <c r="C18" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="25"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="47"/>
-      <c r="L18" s="42"/>
-      <c r="M18" s="48"/>
-      <c r="N18" s="47"/>
-      <c r="O18" s="24"/>
-      <c r="P18" s="48"/>
-      <c r="S18" s="49"/>
-      <c r="T18" s="50"/>
-      <c r="U18" s="51"/>
-      <c r="V18" s="51"/>
-      <c r="W18" s="51"/>
-      <c r="X18" s="51"/>
-      <c r="Y18" s="52"/>
-      <c r="Z18" s="24"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="49"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="50"/>
+      <c r="N18" s="49"/>
+      <c r="O18" s="25"/>
+      <c r="P18" s="50"/>
+      <c r="S18" s="51"/>
+      <c r="T18" s="52"/>
+      <c r="U18" s="53"/>
+      <c r="V18" s="53"/>
+      <c r="W18" s="53"/>
+      <c r="X18" s="53"/>
+      <c r="Y18" s="54"/>
+      <c r="Z18" s="55"/>
     </row>
     <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="43" t="n">
+      <c r="B19" s="44" t="n">
         <v>13</v>
       </c>
-      <c r="C19" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="24"/>
+      <c r="C19" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="25"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="46"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="47"/>
-      <c r="L19" s="42"/>
-      <c r="M19" s="48"/>
-      <c r="N19" s="47"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="48"/>
-      <c r="S19" s="49"/>
-      <c r="T19" s="50"/>
-      <c r="U19" s="51"/>
-      <c r="V19" s="51"/>
-      <c r="W19" s="51"/>
-      <c r="X19" s="51"/>
-      <c r="Y19" s="52"/>
-      <c r="Z19" s="24"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="49"/>
+      <c r="L19" s="46"/>
+      <c r="M19" s="50"/>
+      <c r="N19" s="49"/>
+      <c r="O19" s="25"/>
+      <c r="P19" s="50"/>
+      <c r="S19" s="51"/>
+      <c r="T19" s="52"/>
+      <c r="U19" s="53"/>
+      <c r="V19" s="53"/>
+      <c r="W19" s="53"/>
+      <c r="X19" s="53"/>
+      <c r="Y19" s="54"/>
+      <c r="Z19" s="55"/>
     </row>
     <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="43" t="n">
+      <c r="B20" s="44" t="n">
         <v>14</v>
       </c>
-      <c r="C20" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="24"/>
+      <c r="C20" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="25"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="43"/>
-      <c r="K20" s="47"/>
-      <c r="L20" s="42"/>
-      <c r="M20" s="48"/>
-      <c r="N20" s="47"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="48"/>
-      <c r="S20" s="49"/>
-      <c r="T20" s="50"/>
-      <c r="U20" s="51"/>
-      <c r="V20" s="51"/>
-      <c r="W20" s="51"/>
-      <c r="X20" s="51"/>
-      <c r="Y20" s="52"/>
-      <c r="Z20" s="24"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="44"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="46"/>
+      <c r="M20" s="50"/>
+      <c r="N20" s="49"/>
+      <c r="O20" s="25"/>
+      <c r="P20" s="50"/>
+      <c r="S20" s="51"/>
+      <c r="T20" s="52"/>
+      <c r="U20" s="53"/>
+      <c r="V20" s="53"/>
+      <c r="W20" s="53"/>
+      <c r="X20" s="53"/>
+      <c r="Y20" s="54"/>
+      <c r="Z20" s="55"/>
     </row>
     <row r="21" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="43" t="n">
+      <c r="B21" s="44" t="n">
         <v>15</v>
       </c>
-      <c r="C21" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="24"/>
+      <c r="C21" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="25"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="46"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="42"/>
-      <c r="M21" s="48"/>
-      <c r="N21" s="47"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="48"/>
-      <c r="S21" s="49"/>
-      <c r="T21" s="50"/>
-      <c r="U21" s="51"/>
-      <c r="V21" s="51"/>
-      <c r="W21" s="51"/>
-      <c r="X21" s="51"/>
-      <c r="Y21" s="52"/>
-      <c r="Z21" s="24"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="50"/>
+      <c r="N21" s="49"/>
+      <c r="O21" s="25"/>
+      <c r="P21" s="50"/>
+      <c r="S21" s="51"/>
+      <c r="T21" s="52"/>
+      <c r="U21" s="53"/>
+      <c r="V21" s="53"/>
+      <c r="W21" s="53"/>
+      <c r="X21" s="53"/>
+      <c r="Y21" s="54"/>
+      <c r="Z21" s="55"/>
     </row>
     <row r="22" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="43" t="n">
+      <c r="B22" s="44" t="n">
         <v>16</v>
       </c>
-      <c r="C22" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="24"/>
+      <c r="C22" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="25"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="45"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="47"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="48"/>
-      <c r="N22" s="47"/>
-      <c r="O22" s="24"/>
-      <c r="P22" s="48"/>
-      <c r="S22" s="49"/>
-      <c r="T22" s="50"/>
-      <c r="U22" s="51"/>
-      <c r="V22" s="51"/>
-      <c r="W22" s="51"/>
-      <c r="X22" s="51"/>
-      <c r="Y22" s="52"/>
-      <c r="Z22" s="24"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="50"/>
+      <c r="N22" s="49"/>
+      <c r="O22" s="25"/>
+      <c r="P22" s="50"/>
+      <c r="S22" s="51"/>
+      <c r="T22" s="52"/>
+      <c r="U22" s="53"/>
+      <c r="V22" s="53"/>
+      <c r="W22" s="53"/>
+      <c r="X22" s="53"/>
+      <c r="Y22" s="54"/>
+      <c r="Z22" s="55"/>
     </row>
     <row r="23" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="43" t="n">
+      <c r="B23" s="44" t="n">
         <v>17</v>
       </c>
-      <c r="C23" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="24"/>
+      <c r="C23" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="25"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="43"/>
-      <c r="K23" s="47"/>
-      <c r="L23" s="42"/>
-      <c r="M23" s="48"/>
-      <c r="N23" s="47"/>
-      <c r="O23" s="24"/>
-      <c r="P23" s="48"/>
-      <c r="S23" s="49"/>
-      <c r="T23" s="50"/>
-      <c r="U23" s="51"/>
-      <c r="V23" s="51"/>
-      <c r="W23" s="51"/>
-      <c r="X23" s="51"/>
-      <c r="Y23" s="52"/>
-      <c r="Z23" s="24"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="46"/>
+      <c r="M23" s="50"/>
+      <c r="N23" s="49"/>
+      <c r="O23" s="25"/>
+      <c r="P23" s="50"/>
+      <c r="S23" s="51"/>
+      <c r="T23" s="52"/>
+      <c r="U23" s="53"/>
+      <c r="V23" s="53"/>
+      <c r="W23" s="53"/>
+      <c r="X23" s="53"/>
+      <c r="Y23" s="54"/>
+      <c r="Z23" s="55"/>
     </row>
     <row r="24" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="43" t="n">
+      <c r="B24" s="44" t="n">
         <v>18</v>
       </c>
-      <c r="C24" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="24"/>
+      <c r="C24" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="25"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="46"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="47"/>
-      <c r="L24" s="42"/>
-      <c r="M24" s="48"/>
-      <c r="N24" s="47"/>
-      <c r="O24" s="24"/>
-      <c r="P24" s="48"/>
-      <c r="S24" s="49"/>
-      <c r="T24" s="50"/>
-      <c r="U24" s="51"/>
-      <c r="V24" s="51"/>
-      <c r="W24" s="51"/>
-      <c r="X24" s="51"/>
-      <c r="Y24" s="52"/>
-      <c r="Z24" s="24"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="49"/>
+      <c r="L24" s="46"/>
+      <c r="M24" s="50"/>
+      <c r="N24" s="49"/>
+      <c r="O24" s="25"/>
+      <c r="P24" s="50"/>
+      <c r="S24" s="51"/>
+      <c r="T24" s="52"/>
+      <c r="U24" s="53"/>
+      <c r="V24" s="53"/>
+      <c r="W24" s="53"/>
+      <c r="X24" s="53"/>
+      <c r="Y24" s="54"/>
+      <c r="Z24" s="55"/>
     </row>
     <row r="25" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="43" t="n">
+      <c r="B25" s="44" t="n">
         <v>19</v>
       </c>
-      <c r="C25" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="24"/>
+      <c r="C25" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="25"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="46"/>
-      <c r="J25" s="43"/>
-      <c r="K25" s="47"/>
-      <c r="L25" s="42"/>
-      <c r="M25" s="48"/>
-      <c r="N25" s="47"/>
-      <c r="O25" s="24"/>
-      <c r="P25" s="48"/>
-      <c r="S25" s="49"/>
-      <c r="T25" s="50"/>
-      <c r="U25" s="51"/>
-      <c r="V25" s="51"/>
-      <c r="W25" s="51"/>
-      <c r="X25" s="51"/>
-      <c r="Y25" s="52"/>
-      <c r="Z25" s="24"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="49"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="50"/>
+      <c r="N25" s="49"/>
+      <c r="O25" s="25"/>
+      <c r="P25" s="50"/>
+      <c r="S25" s="51"/>
+      <c r="T25" s="52"/>
+      <c r="U25" s="53"/>
+      <c r="V25" s="53"/>
+      <c r="W25" s="53"/>
+      <c r="X25" s="53"/>
+      <c r="Y25" s="54"/>
+      <c r="Z25" s="55"/>
     </row>
     <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="43" t="n">
+      <c r="B26" s="44" t="n">
         <v>20</v>
       </c>
-      <c r="C26" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="24"/>
+      <c r="C26" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="25"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="46"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="47"/>
-      <c r="L26" s="42"/>
-      <c r="M26" s="48"/>
-      <c r="N26" s="47"/>
-      <c r="O26" s="24"/>
-      <c r="P26" s="48"/>
-      <c r="S26" s="49"/>
-      <c r="T26" s="50"/>
-      <c r="U26" s="51"/>
-      <c r="V26" s="51"/>
-      <c r="W26" s="51"/>
-      <c r="X26" s="51"/>
-      <c r="Y26" s="52"/>
-      <c r="Z26" s="24"/>
+      <c r="H26" s="47"/>
+      <c r="I26" s="48"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="49"/>
+      <c r="L26" s="46"/>
+      <c r="M26" s="50"/>
+      <c r="N26" s="49"/>
+      <c r="O26" s="25"/>
+      <c r="P26" s="50"/>
+      <c r="S26" s="51"/>
+      <c r="T26" s="52"/>
+      <c r="U26" s="53"/>
+      <c r="V26" s="53"/>
+      <c r="W26" s="53"/>
+      <c r="X26" s="53"/>
+      <c r="Y26" s="54"/>
+      <c r="Z26" s="55"/>
     </row>
     <row r="27" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="43" t="n">
+      <c r="B27" s="44" t="n">
         <v>21</v>
       </c>
-      <c r="C27" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="24"/>
+      <c r="C27" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="25"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="46"/>
-      <c r="J27" s="43"/>
-      <c r="K27" s="47"/>
-      <c r="L27" s="42"/>
-      <c r="M27" s="48"/>
-      <c r="N27" s="47"/>
-      <c r="O27" s="24"/>
-      <c r="P27" s="48"/>
-      <c r="S27" s="49"/>
-      <c r="T27" s="50"/>
-      <c r="U27" s="51"/>
-      <c r="V27" s="51"/>
-      <c r="W27" s="51"/>
-      <c r="X27" s="51"/>
-      <c r="Y27" s="52"/>
-      <c r="Z27" s="24"/>
+      <c r="H27" s="47"/>
+      <c r="I27" s="48"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="49"/>
+      <c r="L27" s="46"/>
+      <c r="M27" s="50"/>
+      <c r="N27" s="49"/>
+      <c r="O27" s="25"/>
+      <c r="P27" s="50"/>
+      <c r="S27" s="51"/>
+      <c r="T27" s="52"/>
+      <c r="U27" s="53"/>
+      <c r="V27" s="53"/>
+      <c r="W27" s="53"/>
+      <c r="X27" s="53"/>
+      <c r="Y27" s="54"/>
+      <c r="Z27" s="55"/>
     </row>
     <row r="28" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="43" t="n">
+      <c r="B28" s="44" t="n">
         <v>22</v>
       </c>
-      <c r="C28" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" s="24"/>
+      <c r="C28" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="25"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="46"/>
-      <c r="J28" s="43"/>
-      <c r="K28" s="47"/>
-      <c r="L28" s="42"/>
-      <c r="M28" s="48"/>
-      <c r="N28" s="47"/>
-      <c r="O28" s="24"/>
-      <c r="P28" s="48"/>
-      <c r="S28" s="49"/>
-      <c r="T28" s="50"/>
-      <c r="U28" s="51"/>
-      <c r="V28" s="51"/>
-      <c r="W28" s="51"/>
-      <c r="X28" s="51"/>
-      <c r="Y28" s="52"/>
-      <c r="Z28" s="24"/>
+      <c r="H28" s="47"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="44"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="46"/>
+      <c r="M28" s="50"/>
+      <c r="N28" s="49"/>
+      <c r="O28" s="25"/>
+      <c r="P28" s="50"/>
+      <c r="S28" s="51"/>
+      <c r="T28" s="52"/>
+      <c r="U28" s="53"/>
+      <c r="V28" s="53"/>
+      <c r="W28" s="53"/>
+      <c r="X28" s="53"/>
+      <c r="Y28" s="54"/>
+      <c r="Z28" s="55"/>
     </row>
     <row r="29" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="43" t="n">
+      <c r="B29" s="44" t="n">
         <v>23</v>
       </c>
-      <c r="C29" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" s="24"/>
+      <c r="C29" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="25"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="43"/>
-      <c r="K29" s="47"/>
-      <c r="L29" s="24"/>
-      <c r="M29" s="48"/>
-      <c r="N29" s="47"/>
-      <c r="O29" s="24"/>
-      <c r="P29" s="48"/>
-      <c r="S29" s="49"/>
-      <c r="T29" s="50"/>
-      <c r="U29" s="51"/>
-      <c r="V29" s="51"/>
-      <c r="W29" s="51"/>
-      <c r="X29" s="51"/>
-      <c r="Y29" s="52"/>
-      <c r="Z29" s="24"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="48"/>
+      <c r="J29" s="44"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="25"/>
+      <c r="M29" s="50"/>
+      <c r="N29" s="49"/>
+      <c r="O29" s="25"/>
+      <c r="P29" s="50"/>
+      <c r="S29" s="51"/>
+      <c r="T29" s="52"/>
+      <c r="U29" s="53"/>
+      <c r="V29" s="53"/>
+      <c r="W29" s="53"/>
+      <c r="X29" s="53"/>
+      <c r="Y29" s="54"/>
+      <c r="Z29" s="55"/>
     </row>
     <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="43" t="n">
+      <c r="B30" s="44" t="n">
         <v>24</v>
       </c>
-      <c r="C30" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="24"/>
+      <c r="C30" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="25"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="43"/>
-      <c r="K30" s="47"/>
-      <c r="L30" s="24"/>
-      <c r="M30" s="48"/>
-      <c r="N30" s="47"/>
-      <c r="O30" s="24"/>
-      <c r="P30" s="48"/>
-      <c r="S30" s="49"/>
-      <c r="T30" s="50"/>
-      <c r="U30" s="51"/>
-      <c r="V30" s="51"/>
-      <c r="W30" s="51"/>
-      <c r="X30" s="51"/>
-      <c r="Y30" s="52"/>
-      <c r="Z30" s="24"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="44"/>
+      <c r="K30" s="49"/>
+      <c r="L30" s="25"/>
+      <c r="M30" s="50"/>
+      <c r="N30" s="49"/>
+      <c r="O30" s="25"/>
+      <c r="P30" s="50"/>
+      <c r="S30" s="51"/>
+      <c r="T30" s="52"/>
+      <c r="U30" s="53"/>
+      <c r="V30" s="53"/>
+      <c r="W30" s="53"/>
+      <c r="X30" s="53"/>
+      <c r="Y30" s="54"/>
+      <c r="Z30" s="55"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:Y1"/>
     <mergeCell ref="E2:F2"/>
@@ -2022,6 +2075,7 @@
     <mergeCell ref="N4:P4"/>
     <mergeCell ref="Q4:S4"/>
     <mergeCell ref="T4:Y4"/>
+    <mergeCell ref="Z4:AB4"/>
   </mergeCells>
   <dataValidations count="15">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T6:Y30" type="list">
@@ -2056,7 +2110,7 @@
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6 Z6:AB6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
changes from first remote ops experiment
</commit_message>
<xml_diff>
--- a/startup/wheel_template.xlsx
+++ b/startup/wheel_template.xlsx
@@ -787,9 +787,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1225800</xdr:colOff>
+      <xdr:colOff>1225440</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>59400</xdr:rowOff>
+      <xdr:rowOff>59040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -803,7 +803,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="6933960"/>
-          <a:ext cx="2516400" cy="2742480"/>
+          <a:ext cx="2516040" cy="2742120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -824,9 +824,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>824760</xdr:colOff>
+      <xdr:colOff>824400</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>128520</xdr:rowOff>
+      <xdr:rowOff>128160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -836,7 +836,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3189600" y="6959880"/>
-          <a:ext cx="6644520" cy="1810080"/>
+          <a:ext cx="6644160" cy="1809720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1048,11 +1048,11 @@
   <dimension ref="B1:AMJ30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="6" topLeftCell="O7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="O1" activeCellId="0" sqref="O1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="Z9" activeCellId="0" sqref="Z9"/>
+      <selection pane="bottomRight" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2126,16 +2126,16 @@
       <formula1>-150</formula1>
       <formula2>150</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
-      <formula1>"No,Beginning,End"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G7:G30" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
+      <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>